<commit_message>
added sustainability measures to data(1) (3)
</commit_message>
<xml_diff>
--- a/Data Sets (Excels)/Data (1) (3).xlsx
+++ b/Data Sets (Excels)/Data (1) (3).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofh-my.sharepoint.com/personal/jmfalou_cougarnet_uh_edu/Documents/~Computer Science/z. Hackathon Projects/HalfStackDevs_CodeRedGenesis/Data Sets (Excels)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B116884D-3ADB-43C2-93BC-1D797EACA0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{B116884D-3ADB-43C2-93BC-1D797EACA0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D21E6C06-8729-45D6-ACC2-F6AE7DD725EA}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="6" activeTab="1" xr2:uid="{01528FDC-71FA-430E-A617-D3435C6CD15B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="8" xr2:uid="{01528FDC-71FA-430E-A617-D3435C6CD15B}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,11 @@
     <sheet name="Waste" sheetId="5" r:id="rId6"/>
     <sheet name="Spills" sheetId="6" r:id="rId7"/>
     <sheet name="Production and Facility Info" sheetId="7" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId9"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId10"/>
+  </externalReferences>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="68">
   <si>
     <t>U.S.A.</t>
   </si>
@@ -229,6 +233,24 @@
   </si>
   <si>
     <t>countries</t>
+  </si>
+  <si>
+    <t>GHG Score (Out of 20)</t>
+  </si>
+  <si>
+    <t>Energy Score (Out of 20)</t>
+  </si>
+  <si>
+    <t>Water Score (Out of 20)</t>
+  </si>
+  <si>
+    <t>Waste Score (Out of 20)</t>
+  </si>
+  <si>
+    <t>Spills Score (Out of 20)</t>
+  </si>
+  <si>
+    <t>Sustainability Score (Out of 100)</t>
   </si>
 </sst>
 </file>
@@ -240,7 +262,7 @@
     <numFmt numFmtId="164" formatCode="#,###"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,6 +329,15 @@
       <name val="Calibri Light"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -328,7 +359,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -682,6 +713,201 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -691,7 +917,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
@@ -731,6 +957,23 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -741,25 +984,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{6E9C2E63-9F6E-43C0-BFCD-2DC1E9F19C6C}"/>
@@ -780,6 +1019,193 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="ALL"/>
+      <sheetName val="Sustainability Scores"/>
+      <sheetName val="GHG"/>
+      <sheetName val="Energy"/>
+      <sheetName val="Water"/>
+      <sheetName val="Waste"/>
+      <sheetName val="Spills"/>
+      <sheetName val="Production and Facility Info"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2">
+        <row r="6">
+          <cell r="A6">
+            <v>8440.6803619294606</v>
+          </cell>
+          <cell r="B6">
+            <v>3605.3150430000001</v>
+          </cell>
+          <cell r="C6">
+            <v>1137.9361982912501</v>
+          </cell>
+          <cell r="D6">
+            <v>2830.1430000000005</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>15972.450569727</v>
+          </cell>
+          <cell r="B8">
+            <v>238.91200000000001</v>
+          </cell>
+          <cell r="C8">
+            <v>600.09470903299996</v>
+          </cell>
+          <cell r="D8">
+            <v>1046.51</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>94256.845479921001</v>
+          </cell>
+          <cell r="B9">
+            <v>534.73397999999997</v>
+          </cell>
+          <cell r="C9">
+            <v>3533.33012328</v>
+          </cell>
+          <cell r="D9">
+            <v>182.71</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>42846.268449704003</v>
+          </cell>
+          <cell r="B10">
+            <v>2085.8160600000001</v>
+          </cell>
+          <cell r="C10">
+            <v>1932.696238665</v>
+          </cell>
+          <cell r="D10">
+            <v>1662.99</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>1548.1094865510001</v>
+          </cell>
+          <cell r="B11">
+            <v>929.76693999999998</v>
+          </cell>
+          <cell r="C11">
+            <v>120.18351857499999</v>
+          </cell>
+          <cell r="D11">
+            <v>102.75000000000001</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>1246.1935030069999</v>
+          </cell>
+          <cell r="B12">
+            <v>114.93527</v>
+          </cell>
+          <cell r="C12">
+            <v>78.333718743999995</v>
+          </cell>
+          <cell r="D12">
+            <v>68.400000000000006</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3">
+        <row r="4">
+          <cell r="A4">
+            <v>86.933133434257897</v>
+          </cell>
+          <cell r="B4">
+            <v>60.066288000032003</v>
+          </cell>
+          <cell r="C4">
+            <v>16.857970160000001</v>
+          </cell>
+          <cell r="D4">
+            <v>42.284999999999997</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="2">
+          <cell r="A2">
+            <v>5.4</v>
+          </cell>
+          <cell r="B2">
+            <v>2.1</v>
+          </cell>
+          <cell r="C2">
+            <v>1.6238950000000001</v>
+          </cell>
+          <cell r="D2" t="str">
+            <v>&lt;0.2</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>26.665239999999997</v>
+          </cell>
+          <cell r="B3">
+            <v>0.11321200000000001</v>
+          </cell>
+          <cell r="C3">
+            <v>25.853999999999999</v>
+          </cell>
+          <cell r="D3">
+            <v>1.1000000000000001E-3</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>49.61356</v>
+          </cell>
+          <cell r="B4">
+            <v>24.410564999999998</v>
+          </cell>
+          <cell r="C4">
+            <v>0</v>
+          </cell>
+          <cell r="D4">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>0</v>
+          </cell>
+          <cell r="B5">
+            <v>0</v>
+          </cell>
+          <cell r="C5">
+            <v>129.48417890000002</v>
+          </cell>
+          <cell r="D5">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1085,21 +1511,21 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.85546875" customWidth="1"/>
-    <col min="8" max="8" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.81640625" customWidth="1"/>
+    <col min="8" max="8" width="50.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.600000000000001" thickTop="1" thickBot="1">
+    <row r="1" spans="1:14" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1124,7 +1550,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.6" thickTop="1" thickBot="1">
+    <row r="2" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7">
         <v>6129.1431650302193</v>
       </c>
@@ -1143,7 +1569,7 @@
       <c r="F2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="38" t="s">
         <v>8</v>
       </c>
       <c r="M2" s="8">
@@ -1153,7 +1579,7 @@
         <v>685.36830000000009</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1">
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>710.73203000000001</v>
       </c>
@@ -1172,7 +1598,7 @@
       <c r="F3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="30"/>
+      <c r="G3" s="39"/>
       <c r="M3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1180,7 +1606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1">
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>1592.901827801438</v>
       </c>
@@ -1199,7 +1625,7 @@
       <c r="F4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="30"/>
+      <c r="G4" s="39"/>
       <c r="M4" s="4">
         <v>28.360250000000001</v>
       </c>
@@ -1207,7 +1633,7 @@
         <v>9.9607500000000009</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1">
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>7.9033390978040003</v>
       </c>
@@ -1226,7 +1652,7 @@
       <c r="F5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="30"/>
+      <c r="G5" s="39"/>
       <c r="M5" s="4">
         <v>1.7284000000000002</v>
       </c>
@@ -1234,7 +1660,7 @@
         <v>1.1741199999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1">
+    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>8440.6803619294606</v>
       </c>
@@ -1253,7 +1679,7 @@
       <c r="F6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="30"/>
+      <c r="G6" s="39"/>
       <c r="M6" s="4">
         <v>2133.6398300000005</v>
       </c>
@@ -1261,7 +1687,7 @@
         <v>696.50317000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="26.45" thickBot="1">
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>18.958874153611692</v>
       </c>
@@ -1290,7 +1716,7 @@
         <v>43.26106645962733</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="52.5" thickBot="1">
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>15972.450569727</v>
       </c>
@@ -1319,7 +1745,7 @@
         <v>380.8</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1">
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>94256.845479921001</v>
       </c>
@@ -1338,7 +1764,7 @@
       <c r="F9" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="39" t="s">
         <v>20</v>
       </c>
       <c r="M9" s="4">
@@ -1348,7 +1774,7 @@
         <v>105.59</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1">
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>42846.268449704003</v>
       </c>
@@ -1367,7 +1793,7 @@
       <c r="F10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="30"/>
+      <c r="G10" s="39"/>
       <c r="M10" s="4">
         <v>1193.19</v>
       </c>
@@ -1375,7 +1801,7 @@
         <v>469.8</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1">
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>1548.1094865510001</v>
       </c>
@@ -1394,7 +1820,7 @@
       <c r="F11" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="30"/>
+      <c r="G11" s="39"/>
       <c r="M11" s="4">
         <v>14.73</v>
       </c>
@@ -1402,7 +1828,7 @@
         <v>88.02000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1">
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>1246.1935030069999</v>
       </c>
@@ -1421,7 +1847,7 @@
       <c r="F12" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="30"/>
+      <c r="G12" s="39"/>
       <c r="M12" s="4">
         <v>52</v>
       </c>
@@ -1429,7 +1855,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1">
+    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>81.33</v>
       </c>
@@ -1448,7 +1874,7 @@
       <c r="F13" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="40" t="s">
         <v>25</v>
       </c>
       <c r="M13" s="4">
@@ -1458,7 +1884,7 @@
         <v>4.165</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1">
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>5.6031334342578987</v>
       </c>
@@ -1477,7 +1903,7 @@
       <c r="F14" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="31"/>
+      <c r="G14" s="40"/>
       <c r="M14" s="4">
         <v>0</v>
       </c>
@@ -1485,7 +1911,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1">
+    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>86.933133434257897</v>
       </c>
@@ -1504,7 +1930,7 @@
       <c r="F15" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="31"/>
+      <c r="G15" s="40"/>
       <c r="M15" s="4">
         <v>38.119999999999997</v>
       </c>
@@ -1512,7 +1938,7 @@
         <v>4.165</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1">
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <v>5.4</v>
       </c>
@@ -1531,7 +1957,7 @@
       <c r="F16" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="32" t="s">
+      <c r="G16" s="34" t="s">
         <v>30</v>
       </c>
       <c r="M16" s="4" t="s">
@@ -1541,7 +1967,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" thickBot="1">
+    <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>26.665239999999997</v>
       </c>
@@ -1560,7 +1986,7 @@
       <c r="F17" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="32"/>
+      <c r="G17" s="34"/>
       <c r="M17" s="4">
         <v>0</v>
       </c>
@@ -1568,7 +1994,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15" thickBot="1">
+    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>49.61356</v>
       </c>
@@ -1587,7 +2013,7 @@
       <c r="F18" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="32"/>
+      <c r="G18" s="34"/>
       <c r="M18" s="4">
         <v>0</v>
       </c>
@@ -1595,7 +2021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15" thickBot="1">
+    <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <v>0</v>
       </c>
@@ -1614,7 +2040,7 @@
       <c r="F19" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="32"/>
+      <c r="G19" s="34"/>
       <c r="M19" s="4">
         <v>0</v>
       </c>
@@ -1622,7 +2048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15" thickBot="1">
+    <row r="20" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <v>1</v>
       </c>
@@ -1641,7 +2067,7 @@
       <c r="F20" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="G20" s="41" t="s">
         <v>36</v>
       </c>
       <c r="M20" s="4">
@@ -1651,7 +2077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15" thickBot="1">
+    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <v>195</v>
       </c>
@@ -1670,7 +2096,7 @@
       <c r="F21" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="33"/>
+      <c r="G21" s="41"/>
       <c r="M21" s="4">
         <v>0</v>
       </c>
@@ -1678,7 +2104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15" thickBot="1">
+    <row r="22" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>96</v>
       </c>
@@ -1697,7 +2123,7 @@
       <c r="F22" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="33"/>
+      <c r="G22" s="41"/>
       <c r="M22" s="4">
         <v>0</v>
       </c>
@@ -1705,7 +2131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15" thickBot="1">
+    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>749</v>
       </c>
@@ -1724,7 +2150,7 @@
       <c r="F23" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="33"/>
+      <c r="G23" s="41"/>
       <c r="M23" s="4">
         <v>0</v>
       </c>
@@ -1732,7 +2158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15" thickBot="1">
+    <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>390</v>
       </c>
@@ -1751,7 +2177,7 @@
       <c r="F24" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="33"/>
+      <c r="G24" s="41"/>
       <c r="M24" s="4">
         <v>0</v>
       </c>
@@ -1759,7 +2185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15" thickBot="1">
+    <row r="25" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3">
         <v>23.32</v>
       </c>
@@ -1778,7 +2204,7 @@
       <c r="F25" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="G25" s="32" t="s">
+      <c r="G25" s="34" t="s">
         <v>42</v>
       </c>
       <c r="M25" s="4">
@@ -1788,7 +2214,7 @@
         <v>240.92</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15" thickBot="1">
+    <row r="26" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>197546.25</v>
       </c>
@@ -1807,7 +2233,7 @@
       <c r="F26" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="32"/>
+      <c r="G26" s="34"/>
       <c r="M26" s="4">
         <v>144.52000000000001</v>
       </c>
@@ -1815,7 +2241,7 @@
         <v>129.26300000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15" thickBot="1">
+    <row r="27" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>252483.16</v>
       </c>
@@ -1834,7 +2260,7 @@
       <c r="F27" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G27" s="32"/>
+      <c r="G27" s="34"/>
       <c r="M27" s="4">
         <v>518.64</v>
       </c>
@@ -1842,7 +2268,7 @@
         <v>25.83</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15" thickBot="1">
+    <row r="28" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>450052.73</v>
       </c>
@@ -1861,7 +2287,7 @@
       <c r="F28" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G28" s="32"/>
+      <c r="G28" s="34"/>
       <c r="M28" s="4">
         <v>667.57999999999993</v>
       </c>
@@ -1869,7 +2295,7 @@
         <v>396.01299999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15" thickBot="1">
+    <row r="29" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="3">
         <v>197569.57</v>
       </c>
@@ -1888,7 +2314,7 @@
       <c r="F29" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G29" s="32"/>
+      <c r="G29" s="34"/>
       <c r="M29" s="4">
         <v>148.94</v>
       </c>
@@ -1896,7 +2322,7 @@
         <v>370.18299999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15" thickBot="1">
+    <row r="30" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3">
         <v>445.21</v>
       </c>
@@ -1925,7 +2351,7 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15" thickBot="1">
+    <row r="31" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="7">
         <f>989+200</f>
         <v>1189</v>
@@ -1950,7 +2376,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15" thickBot="1">
+    <row r="32" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3">
         <f>3+1.5</f>
         <v>4.5</v>
@@ -1975,7 +2401,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15" thickBot="1">
+    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3">
         <f>5.6+1.1</f>
         <v>6.6999999999999993</v>
@@ -2000,7 +2426,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15" thickBot="1">
+    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3">
         <f>10.3+1.8</f>
         <v>12.100000000000001</v>
@@ -2025,7 +2451,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15" thickBot="1">
+    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3">
         <v>2</v>
       </c>
@@ -2045,11 +2471,11 @@
       <c r="F35" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="G35" s="34" t="s">
+      <c r="G35" s="35" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15" thickBot="1">
+    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3">
         <v>7</v>
       </c>
@@ -2069,9 +2495,9 @@
       <c r="F36" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G36" s="35"/>
-    </row>
-    <row r="37" spans="1:9" ht="15" thickBot="1">
+      <c r="G36" s="36"/>
+    </row>
+    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="5">
         <v>3</v>
       </c>
@@ -2091,13 +2517,13 @@
       <c r="F37" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="G37" s="36"/>
-    </row>
-    <row r="38" spans="1:9" ht="15" thickTop="1">
+      <c r="G37" s="37"/>
+    </row>
+    <row r="38" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="H38" s="1"/>
       <c r="I38" s="16"/>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2107,7 +2533,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="16"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2136,45 +2562,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1904851B-1F9A-45D7-B557-1A55394C9595}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="18.75">
-      <c r="A2" s="37" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="18.75">
-      <c r="A3" s="38" t="s">
+    <row r="2" spans="1:1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="30" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="18.75">
-      <c r="A4" s="38" t="s">
+    <row r="4" spans="1:1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="30" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="18.75">
-      <c r="A5" s="38" t="s">
+    <row r="5" spans="1:1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="30" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="40"/>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="41"/>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="32"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2189,18 +2615,18 @@
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="50.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75">
+    <row r="1" spans="1:7" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A1" s="15"/>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -2219,7 +2645,7 @@
       </c>
       <c r="G1" s="16"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>7</v>
       </c>
@@ -2238,11 +2664,11 @@
       <c r="F2" s="12">
         <v>13228.247138200219</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="38" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
@@ -2261,9 +2687,9 @@
       <c r="F3" s="13">
         <v>1059.88886</v>
       </c>
-      <c r="G3" s="30"/>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="G3" s="39"/>
+    </row>
+    <row r="4" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>12</v>
       </c>
@@ -2282,9 +2708,9 @@
       <c r="F4" s="13">
         <v>1704.4953379226879</v>
       </c>
-      <c r="G4" s="30"/>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="G4" s="39"/>
+    </row>
+    <row r="5" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>13</v>
       </c>
@@ -2303,9 +2729,9 @@
       <c r="F5" s="13">
         <v>21.443267097804</v>
       </c>
-      <c r="G5" s="30"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5" s="39"/>
+    </row>
+    <row r="6" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>14</v>
       </c>
@@ -2324,9 +2750,9 @@
       <c r="F6" s="13">
         <v>16014.07460322071</v>
       </c>
-      <c r="G6" s="30"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6" s="39"/>
+    </row>
+    <row r="7" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>15</v>
       </c>
@@ -2349,7 +2775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>17</v>
       </c>
@@ -2372,7 +2798,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="21" t="s">
         <v>19</v>
       </c>
@@ -2391,11 +2817,11 @@
       <c r="F9" s="13">
         <v>98507.619583200998</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="39" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
         <v>21</v>
       </c>
@@ -2414,9 +2840,9 @@
       <c r="F10" s="13">
         <v>48527.770748369003</v>
       </c>
-      <c r="G10" s="30"/>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="G10" s="39"/>
+    </row>
+    <row r="11" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
         <v>22</v>
       </c>
@@ -2435,9 +2861,9 @@
       <c r="F11" s="13">
         <v>2700.809945126</v>
       </c>
-      <c r="G11" s="30"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="G11" s="39"/>
+    </row>
+    <row r="12" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>23</v>
       </c>
@@ -2456,9 +2882,9 @@
       <c r="F12" s="13">
         <v>1507.8624917509999</v>
       </c>
-      <c r="G12" s="30"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="G12" s="39"/>
+    </row>
+    <row r="13" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2466,7 +2892,7 @@
       <c r="E13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2492,19 +2918,19 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7265625" customWidth="1"/>
+    <col min="8" max="8" width="24.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75">
+    <row r="1" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A1" s="15"/>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -2523,7 +2949,7 @@
       </c>
       <c r="H1" s="16"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>24</v>
       </c>
@@ -2542,11 +2968,11 @@
       <c r="F2" s="13">
         <v>198.74997016</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="40" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>26</v>
       </c>
@@ -2565,9 +2991,9 @@
       <c r="F3" s="13">
         <v>7.3924214342898988</v>
       </c>
-      <c r="G3" s="31"/>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="G3" s="40"/>
+    </row>
+    <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>27</v>
       </c>
@@ -2586,9 +3012,9 @@
       <c r="F4" s="13">
         <v>206.1423915942899</v>
       </c>
-      <c r="G4" s="31"/>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="G4" s="40"/>
+    </row>
+    <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2596,7 +3022,7 @@
       <c r="E5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2621,19 +3047,19 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.81640625" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75">
+    <row r="1" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A1" s="15"/>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -2652,7 +3078,7 @@
       </c>
       <c r="H1" s="16"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
         <v>29</v>
       </c>
@@ -2671,11 +3097,11 @@
       <c r="F2" s="13">
         <v>9.2238950000000006</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="34" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="23" t="s">
         <v>32</v>
       </c>
@@ -2694,9 +3120,9 @@
       <c r="F3" s="13">
         <v>52.633552000000002</v>
       </c>
-      <c r="G3" s="32"/>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="G3" s="34"/>
+    </row>
+    <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="23" t="s">
         <v>33</v>
       </c>
@@ -2715,9 +3141,9 @@
       <c r="F4" s="13">
         <v>74.024124999999998</v>
       </c>
-      <c r="G4" s="32"/>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="G4" s="34"/>
+    </row>
+    <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
         <v>34</v>
       </c>
@@ -2736,9 +3162,9 @@
       <c r="F5" s="13">
         <v>129.48417890000002</v>
       </c>
-      <c r="G5" s="32"/>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="G5" s="34"/>
+    </row>
+    <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2763,19 +3189,19 @@
       <selection activeCell="G2" sqref="G2:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.1796875" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75">
+    <row r="1" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A1" s="15"/>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -2794,7 +3220,7 @@
       </c>
       <c r="H1" s="16"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
         <v>41</v>
       </c>
@@ -2813,11 +3239,11 @@
       <c r="F2" s="13">
         <v>78599.760600000009</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="34" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="23" t="s">
         <v>43</v>
       </c>
@@ -2836,9 +3262,9 @@
       <c r="F3" s="13">
         <v>322488.61666</v>
       </c>
-      <c r="G3" s="32"/>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="G3" s="34"/>
+    </row>
+    <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>44</v>
       </c>
@@ -2857,9 +3283,9 @@
       <c r="F4" s="13">
         <v>265507.54095000005</v>
       </c>
-      <c r="G4" s="32"/>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="G4" s="34"/>
+    </row>
+    <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>45</v>
       </c>
@@ -2878,9 +3304,9 @@
       <c r="F5" s="13">
         <v>666595.91821000003</v>
       </c>
-      <c r="G5" s="32"/>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="G5" s="34"/>
+    </row>
+    <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>46</v>
       </c>
@@ -2899,9 +3325,9 @@
       <c r="F6" s="13">
         <v>401088.37725999998</v>
       </c>
-      <c r="G6" s="32"/>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="G6" s="34"/>
+    </row>
+    <row r="7" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2909,7 +3335,7 @@
       <c r="E7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2934,18 +3360,18 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="48.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" customWidth="1"/>
-    <col min="6" max="6" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.81640625" customWidth="1"/>
+    <col min="6" max="6" width="47.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75">
+    <row r="1" spans="1:7" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A1" s="15"/>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -2964,7 +3390,7 @@
       </c>
       <c r="G1" s="16"/>
     </row>
-    <row r="2" spans="1:7" ht="15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
         <v>35</v>
       </c>
@@ -2983,11 +3409,11 @@
       <c r="F2" s="13">
         <v>2</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="41" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="23" t="s">
         <v>37</v>
       </c>
@@ -3006,9 +3432,9 @@
       <c r="F3" s="13">
         <v>299</v>
       </c>
-      <c r="G3" s="33"/>
-    </row>
-    <row r="4" spans="1:7" ht="15">
+      <c r="G3" s="41"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="23" t="s">
         <v>38</v>
       </c>
@@ -3027,9 +3453,9 @@
       <c r="F4" s="13">
         <v>99</v>
       </c>
-      <c r="G4" s="33"/>
-    </row>
-    <row r="5" spans="1:7" ht="15">
+      <c r="G4" s="41"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
         <v>39</v>
       </c>
@@ -3048,9 +3474,9 @@
       <c r="F5" s="13">
         <v>861</v>
       </c>
-      <c r="G5" s="33"/>
-    </row>
-    <row r="6" spans="1:7" ht="15">
+      <c r="G5" s="41"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="23" t="s">
         <v>40</v>
       </c>
@@ -3069,9 +3495,9 @@
       <c r="F6" s="13">
         <v>496</v>
       </c>
-      <c r="G6" s="33"/>
-    </row>
-    <row r="7" spans="1:7" ht="15">
+      <c r="G6" s="41"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3079,7 +3505,7 @@
       <c r="E7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3104,18 +3530,18 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75">
+    <row r="1" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A1" s="15"/>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -3134,7 +3560,7 @@
       </c>
       <c r="G1" s="16"/>
     </row>
-    <row r="2" spans="1:8" ht="15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>47</v>
       </c>
@@ -3157,7 +3583,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>49</v>
       </c>
@@ -3182,7 +3608,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>51</v>
       </c>
@@ -3207,7 +3633,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>53</v>
       </c>
@@ -3232,7 +3658,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>55</v>
       </c>
@@ -3257,7 +3683,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>57</v>
       </c>
@@ -3277,11 +3703,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="35" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>59</v>
       </c>
@@ -3301,9 +3727,9 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G8" s="35"/>
-    </row>
-    <row r="9" spans="1:8" ht="15">
+      <c r="G8" s="36"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="24" t="s">
         <v>60</v>
       </c>
@@ -3323,12 +3749,12 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="G9" s="36"/>
-    </row>
-    <row r="10" spans="1:8" ht="15">
+      <c r="G9" s="37"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -3337,7 +3763,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -3353,4 +3779,143 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD8AEB7-D2E8-4525-A681-2676EB3834C0}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="46">
+        <f xml:space="preserve"> 20000 / [1]GHG!A6 + 2000 / SUM( [1]GHG!A8:A12)</f>
+        <v>2.3823084554870104</v>
+      </c>
+      <c r="C2" s="46">
+        <f xml:space="preserve"> 20000 / [1]GHG!B6 + 2000 / SUM( [1]GHG!B8:B12)</f>
+        <v>6.0596389501013492</v>
+      </c>
+      <c r="D2" s="46">
+        <f xml:space="preserve"> 20000 / [1]GHG!C6 + 2000 / SUM( [1]GHG!C8:C12)</f>
+        <v>17.894930089120145</v>
+      </c>
+      <c r="E2" s="46">
+        <f xml:space="preserve"> 20000 / [1]GHG!D6 + 2000 / SUM( [1]GHG!D8:D12)</f>
+        <v>7.719658610227814</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="48">
+        <f>333 / [1]Energy!A4</f>
+        <v>3.8305302805152781</v>
+      </c>
+      <c r="C3" s="48">
+        <f>333 / [1]Energy!B4</f>
+        <v>5.5438751267570021</v>
+      </c>
+      <c r="D3" s="48">
+        <f>333 / [1]Energy!C4</f>
+        <v>19.753267851317634</v>
+      </c>
+      <c r="E3" s="48">
+        <f>333 / [1]Energy!D4</f>
+        <v>7.8751330258957086</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="48">
+        <f>1 / SUM([1]Water!A2:A3) + [1]Water!A4 / 1000 + 5 / ([1]Water!A5 + 1)</f>
+        <v>5.0807999786888978</v>
+      </c>
+      <c r="C4" s="48">
+        <f>1 / SUM([1]Water!B2:B3) + [1]Water!B4 / 1000 + 5 / ([1]Water!B5 + 1)</f>
+        <v>5.4762425630191682</v>
+      </c>
+      <c r="D4" s="48">
+        <f>1 / SUM([1]Water!C2:C3) + [1]Water!C4 / 1000 + 5 / ([1]Water!C5 + 1)</f>
+        <v>7.4711711437762368E-2</v>
+      </c>
+      <c r="E4" s="48">
+        <f>1 / SUM([1]Water!D2:D3) + [1]Water!D4 / 1000 + 5 / ([1]Water!D5 + 1)</f>
+        <v>914.09090909090901</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="49"/>
+    </row>
+    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="52"/>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="54">
+        <f>SUM(B2:B6)</f>
+        <v>11.293638714691186</v>
+      </c>
+      <c r="C7" s="54">
+        <f t="shared" ref="C7:E7" si="0">SUM(C2:C6)</f>
+        <v>17.07975663987752</v>
+      </c>
+      <c r="D7" s="54">
+        <f t="shared" si="0"/>
+        <v>37.722909651875547</v>
+      </c>
+      <c r="E7" s="54">
+        <f t="shared" si="0"/>
+        <v>929.68570072703255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
made uniform units for the GHG and WATER sheets in data.xlsx
</commit_message>
<xml_diff>
--- a/Data Sets (Excels)/Data (1) (3).xlsx
+++ b/Data Sets (Excels)/Data (1) (3).xlsx
@@ -8,23 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofh-my.sharepoint.com/personal/jmfalou_cougarnet_uh_edu/Documents/~Computer Science/z. Hackathon Projects/HalfStackDevs_CodeRedGenesis/Data Sets (Excels)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{B116884D-3ADB-43C2-93BC-1D797EACA0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D21E6C06-8729-45D6-ACC2-F6AE7DD725EA}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{B116884D-3ADB-43C2-93BC-1D797EACA0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5111178C-C32A-405B-84E6-699AF57D58E3}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="8" xr2:uid="{01528FDC-71FA-430E-A617-D3435C6CD15B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="2" activeTab="3" xr2:uid="{01528FDC-71FA-430E-A617-D3435C6CD15B}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="8" r:id="rId2"/>
     <sheet name="GHG" sheetId="2" r:id="rId3"/>
-    <sheet name="Energy" sheetId="3" r:id="rId4"/>
-    <sheet name="Water" sheetId="4" r:id="rId5"/>
-    <sheet name="Waste" sheetId="5" r:id="rId6"/>
-    <sheet name="Spills" sheetId="6" r:id="rId7"/>
-    <sheet name="Production and Facility Info" sheetId="7" r:id="rId8"/>
-    <sheet name="Sheet2" sheetId="9" r:id="rId9"/>
+    <sheet name="GHG (Uniform Units)" sheetId="10" r:id="rId4"/>
+    <sheet name="Energy" sheetId="3" r:id="rId5"/>
+    <sheet name="Water" sheetId="4" r:id="rId6"/>
+    <sheet name="Water (Uniform Units)" sheetId="11" r:id="rId7"/>
+    <sheet name="Waste" sheetId="5" r:id="rId8"/>
+    <sheet name="Spills" sheetId="6" r:id="rId9"/>
+    <sheet name="Production and Facility Info" sheetId="7" r:id="rId10"/>
+    <sheet name="Sustainability Scores" sheetId="9" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <calcPr calcId="191028"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="74">
   <si>
     <t>U.S.A.</t>
   </si>
@@ -251,6 +253,24 @@
   </si>
   <si>
     <t>Sustainability Score (Out of 100)</t>
+  </si>
+  <si>
+    <t>GHGs (tonnes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Hydrocarbons in Overboard Discharges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Produced Water Recycle/Reuse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Non-Fresh Water Withdrawn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Fresh Water Withdrawn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tonnes </t>
   </si>
 </sst>
 </file>
@@ -359,7 +379,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -901,6 +921,185 @@
         <color auto="1"/>
       </right>
       <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="thick">
@@ -917,7 +1116,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
@@ -962,6 +1161,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -986,19 +1198,24 @@
     <xf numFmtId="165" fontId="5" fillId="3" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="40" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="41" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="42" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="43" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="5" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{6E9C2E63-9F6E-43C0-BFCD-2DC1E9F19C6C}"/>
@@ -1206,6 +1423,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1569,7 +1790,7 @@
       <c r="F2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="51" t="s">
         <v>8</v>
       </c>
       <c r="M2" s="8">
@@ -1598,7 +1819,7 @@
       <c r="F3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="39"/>
+      <c r="G3" s="52"/>
       <c r="M3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1625,7 +1846,7 @@
       <c r="F4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="39"/>
+      <c r="G4" s="52"/>
       <c r="M4" s="4">
         <v>28.360250000000001</v>
       </c>
@@ -1652,7 +1873,7 @@
       <c r="F5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="39"/>
+      <c r="G5" s="52"/>
       <c r="M5" s="4">
         <v>1.7284000000000002</v>
       </c>
@@ -1679,7 +1900,7 @@
       <c r="F6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="39"/>
+      <c r="G6" s="52"/>
       <c r="M6" s="4">
         <v>2133.6398300000005</v>
       </c>
@@ -1764,7 +1985,7 @@
       <c r="F9" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="52" t="s">
         <v>20</v>
       </c>
       <c r="M9" s="4">
@@ -1793,7 +2014,7 @@
       <c r="F10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="39"/>
+      <c r="G10" s="52"/>
       <c r="M10" s="4">
         <v>1193.19</v>
       </c>
@@ -1820,7 +2041,7 @@
       <c r="F11" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="39"/>
+      <c r="G11" s="52"/>
       <c r="M11" s="4">
         <v>14.73</v>
       </c>
@@ -1847,7 +2068,7 @@
       <c r="F12" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="39"/>
+      <c r="G12" s="52"/>
       <c r="M12" s="4">
         <v>52</v>
       </c>
@@ -1874,7 +2095,7 @@
       <c r="F13" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="40" t="s">
+      <c r="G13" s="53" t="s">
         <v>25</v>
       </c>
       <c r="M13" s="4">
@@ -1903,7 +2124,7 @@
       <c r="F14" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="40"/>
+      <c r="G14" s="53"/>
       <c r="M14" s="4">
         <v>0</v>
       </c>
@@ -1930,7 +2151,7 @@
       <c r="F15" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="40"/>
+      <c r="G15" s="53"/>
       <c r="M15" s="4">
         <v>38.119999999999997</v>
       </c>
@@ -1957,7 +2178,7 @@
       <c r="F16" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="34" t="s">
+      <c r="G16" s="47" t="s">
         <v>30</v>
       </c>
       <c r="M16" s="4" t="s">
@@ -1986,7 +2207,7 @@
       <c r="F17" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="34"/>
+      <c r="G17" s="47"/>
       <c r="M17" s="4">
         <v>0</v>
       </c>
@@ -2013,7 +2234,7 @@
       <c r="F18" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="34"/>
+      <c r="G18" s="47"/>
       <c r="M18" s="4">
         <v>0</v>
       </c>
@@ -2040,7 +2261,7 @@
       <c r="F19" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="34"/>
+      <c r="G19" s="47"/>
       <c r="M19" s="4">
         <v>0</v>
       </c>
@@ -2067,7 +2288,7 @@
       <c r="F20" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="41" t="s">
+      <c r="G20" s="54" t="s">
         <v>36</v>
       </c>
       <c r="M20" s="4">
@@ -2096,7 +2317,7 @@
       <c r="F21" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="41"/>
+      <c r="G21" s="54"/>
       <c r="M21" s="4">
         <v>0</v>
       </c>
@@ -2123,7 +2344,7 @@
       <c r="F22" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="41"/>
+      <c r="G22" s="54"/>
       <c r="M22" s="4">
         <v>0</v>
       </c>
@@ -2150,7 +2371,7 @@
       <c r="F23" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="41"/>
+      <c r="G23" s="54"/>
       <c r="M23" s="4">
         <v>0</v>
       </c>
@@ -2177,7 +2398,7 @@
       <c r="F24" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="41"/>
+      <c r="G24" s="54"/>
       <c r="M24" s="4">
         <v>0</v>
       </c>
@@ -2204,7 +2425,7 @@
       <c r="F25" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="G25" s="34" t="s">
+      <c r="G25" s="47" t="s">
         <v>42</v>
       </c>
       <c r="M25" s="4">
@@ -2233,7 +2454,7 @@
       <c r="F26" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="34"/>
+      <c r="G26" s="47"/>
       <c r="M26" s="4">
         <v>144.52000000000001</v>
       </c>
@@ -2260,7 +2481,7 @@
       <c r="F27" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G27" s="34"/>
+      <c r="G27" s="47"/>
       <c r="M27" s="4">
         <v>518.64</v>
       </c>
@@ -2287,7 +2508,7 @@
       <c r="F28" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G28" s="34"/>
+      <c r="G28" s="47"/>
       <c r="M28" s="4">
         <v>667.57999999999993</v>
       </c>
@@ -2314,7 +2535,7 @@
       <c r="F29" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G29" s="34"/>
+      <c r="G29" s="47"/>
       <c r="M29" s="4">
         <v>148.94</v>
       </c>
@@ -2471,7 +2692,7 @@
       <c r="F35" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="G35" s="35" t="s">
+      <c r="G35" s="48" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2495,7 +2716,7 @@
       <c r="F36" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G36" s="36"/>
+      <c r="G36" s="49"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="5">
@@ -2517,7 +2738,7 @@
       <c r="F37" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="G37" s="37"/>
+      <c r="G37" s="50"/>
     </row>
     <row r="38" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="H38" s="1"/>
@@ -2554,6 +2775,404 @@
     <mergeCell ref="G16:G19"/>
     <mergeCell ref="G20:G24"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C4FF68-BC2E-4B44-9D83-60450A12F19E}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView zoomScale="110" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="45.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="15"/>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="16"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3">
+        <v>445.21</v>
+      </c>
+      <c r="C2" s="4">
+        <v>64.026368000000005</v>
+      </c>
+      <c r="D2" s="4">
+        <v>80.385821050000004</v>
+      </c>
+      <c r="E2" s="4">
+        <v>98.66</v>
+      </c>
+      <c r="F2" s="13">
+        <v>688.28218905000006</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="7">
+        <f>989+200</f>
+        <v>1189</v>
+      </c>
+      <c r="C3" s="8">
+        <v>85</v>
+      </c>
+      <c r="D3" s="8">
+        <v>248</v>
+      </c>
+      <c r="E3" s="12">
+        <v>216</v>
+      </c>
+      <c r="F3" s="27">
+        <f>SUM(B3:E3)</f>
+        <v>1738</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="3">
+        <f>3+1.5</f>
+        <v>4.5</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="F4" s="27">
+        <f t="shared" ref="F4:F9" si="0">SUM(B4:E4)</f>
+        <v>5.4</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="3">
+        <f>5.6+1.1</f>
+        <v>6.6999999999999993</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="13">
+        <v>1.9</v>
+      </c>
+      <c r="F5" s="27">
+        <f t="shared" si="0"/>
+        <v>10.1</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="3">
+        <f>10.3+1.8</f>
+        <v>12.100000000000001</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="E6" s="13">
+        <v>7.1</v>
+      </c>
+      <c r="F6" s="27">
+        <f t="shared" si="0"/>
+        <v>24.6</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3</v>
+      </c>
+      <c r="E7" s="13">
+        <v>3</v>
+      </c>
+      <c r="F7" s="27">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="G7" s="48" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="3">
+        <v>7</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>6</v>
+      </c>
+      <c r="E8" s="13">
+        <v>5</v>
+      </c>
+      <c r="F8" s="27">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G8" s="49"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="5">
+        <v>3</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6">
+        <v>5</v>
+      </c>
+      <c r="E9" s="14">
+        <v>4</v>
+      </c>
+      <c r="F9" s="28">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G9" s="50"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G7:G9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD8AEB7-D2E8-4525-A681-2676EB3834C0}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="38">
+        <f xml:space="preserve"> 20000 / [1]GHG!A6 + 2000 / SUM( [1]GHG!A8:A12)</f>
+        <v>2.3823084554870104</v>
+      </c>
+      <c r="C2" s="38">
+        <f xml:space="preserve"> 20000 / [1]GHG!B6 + 2000 / SUM( [1]GHG!B8:B12)</f>
+        <v>6.0596389501013492</v>
+      </c>
+      <c r="D2" s="38">
+        <f xml:space="preserve"> 20000 / [1]GHG!C6 + 2000 / SUM( [1]GHG!C8:C12)</f>
+        <v>17.894930089120145</v>
+      </c>
+      <c r="E2" s="38">
+        <f xml:space="preserve"> 20000 / [1]GHG!D6 + 2000 / SUM( [1]GHG!D8:D12)</f>
+        <v>7.719658610227814</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="40">
+        <f>333 / [1]Energy!A4</f>
+        <v>3.8305302805152781</v>
+      </c>
+      <c r="C3" s="40">
+        <f>333 / [1]Energy!B4</f>
+        <v>5.5438751267570021</v>
+      </c>
+      <c r="D3" s="40">
+        <f>333 / [1]Energy!C4</f>
+        <v>19.753267851317634</v>
+      </c>
+      <c r="E3" s="40">
+        <f>333 / [1]Energy!D4</f>
+        <v>7.8751330258957086</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="40">
+        <f>1 / SUM([1]Water!A2:A3) + [1]Water!A4 / 1000 + 5 / ([1]Water!A5 + 1)</f>
+        <v>5.0807999786888978</v>
+      </c>
+      <c r="C4" s="40">
+        <f>1 / SUM([1]Water!B2:B3) + [1]Water!B4 / 1000 + 5 / ([1]Water!B5 + 1)</f>
+        <v>5.4762425630191682</v>
+      </c>
+      <c r="D4" s="40">
+        <f>1 / SUM([1]Water!C2:C3) + [1]Water!C4 / 1000 + 5 / ([1]Water!C5 + 1)</f>
+        <v>7.4711711437762368E-2</v>
+      </c>
+      <c r="E4" s="40">
+        <f>1 / SUM([1]Water!D2:D3) + [1]Water!D4 / 1000 + 5 / ([1]Water!D5 + 1)</f>
+        <v>914.09090909090901</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="41"/>
+    </row>
+    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="44"/>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="46">
+        <f>SUM(B2:B6)</f>
+        <v>11.293638714691186</v>
+      </c>
+      <c r="C7" s="46">
+        <f t="shared" ref="C7:E7" si="0">SUM(C2:C6)</f>
+        <v>17.07975663987752</v>
+      </c>
+      <c r="D7" s="46">
+        <f t="shared" si="0"/>
+        <v>37.722909651875547</v>
+      </c>
+      <c r="E7" s="46">
+        <f t="shared" si="0"/>
+        <v>929.68570072703255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2611,8 +3230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36DA8A9C-7F0B-48FD-A6B9-A601A5AB1BB5}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView zoomScale="83" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2664,7 +3283,7 @@
       <c r="F2" s="12">
         <v>13228.247138200219</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="51" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2687,7 +3306,7 @@
       <c r="F3" s="13">
         <v>1059.88886</v>
       </c>
-      <c r="G3" s="39"/>
+      <c r="G3" s="52"/>
     </row>
     <row r="4" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
@@ -2708,7 +3327,7 @@
       <c r="F4" s="13">
         <v>1704.4953379226879</v>
       </c>
-      <c r="G4" s="39"/>
+      <c r="G4" s="52"/>
     </row>
     <row r="5" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
@@ -2729,7 +3348,7 @@
       <c r="F5" s="13">
         <v>21.443267097804</v>
       </c>
-      <c r="G5" s="39"/>
+      <c r="G5" s="52"/>
     </row>
     <row r="6" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
@@ -2750,7 +3369,7 @@
       <c r="F6" s="13">
         <v>16014.07460322071</v>
       </c>
-      <c r="G6" s="39"/>
+      <c r="G6" s="52"/>
     </row>
     <row r="7" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
@@ -2817,7 +3436,7 @@
       <c r="F9" s="13">
         <v>98507.619583200998</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="52" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2840,7 +3459,7 @@
       <c r="F10" s="13">
         <v>48527.770748369003</v>
       </c>
-      <c r="G10" s="39"/>
+      <c r="G10" s="52"/>
     </row>
     <row r="11" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
@@ -2861,7 +3480,7 @@
       <c r="F11" s="13">
         <v>2700.809945126</v>
       </c>
-      <c r="G11" s="39"/>
+      <c r="G11" s="52"/>
     </row>
     <row r="12" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
@@ -2882,7 +3501,7 @@
       <c r="F12" s="13">
         <v>1507.8624917509999</v>
       </c>
-      <c r="G12" s="39"/>
+      <c r="G12" s="52"/>
     </row>
     <row r="13" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
@@ -2911,11 +3530,292 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B11A20-252D-4AB9-80BE-AA57F15F88DC}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="34.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="15"/>
+      <c r="B1" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="59" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="16"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="60">
+        <f>GHG!B2 * 1000</f>
+        <v>6129143.1650302196</v>
+      </c>
+      <c r="C2" s="61">
+        <f>GHG!C2 * 1000</f>
+        <v>3216656.88</v>
+      </c>
+      <c r="D2" s="61">
+        <f>GHG!D2 * 1000</f>
+        <v>1093527.61317</v>
+      </c>
+      <c r="E2" s="61">
+        <f>GHG!E2 * 1000</f>
+        <v>2788919.4800000004</v>
+      </c>
+      <c r="F2" s="62">
+        <f>GHG!F2 * 1000</f>
+        <v>13228247.138200218</v>
+      </c>
+      <c r="G2" s="55" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="63">
+        <f>GHG!B3 * 1000</f>
+        <v>710732.03</v>
+      </c>
+      <c r="C3" s="64">
+        <f>GHG!C3 * 1000</f>
+        <v>335608.83</v>
+      </c>
+      <c r="D3" s="64">
+        <f>GHG!D3 * 1000</f>
+        <v>13548</v>
+      </c>
+      <c r="E3" s="64">
+        <f>GHG!E3 * 1000</f>
+        <v>900</v>
+      </c>
+      <c r="F3" s="65">
+        <f>GHG!F3 * 1000</f>
+        <v>1059888.8600000001</v>
+      </c>
+      <c r="G3" s="56"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="63">
+        <f>GHG!B4 * 1000</f>
+        <v>1592901.827801438</v>
+      </c>
+      <c r="C4" s="64">
+        <f>GHG!C4 * 1000</f>
+        <v>46285.925000000003</v>
+      </c>
+      <c r="D4" s="64">
+        <f>GHG!D4 * 1000</f>
+        <v>26986.585121249998</v>
+      </c>
+      <c r="E4" s="64">
+        <f>GHG!E4 * 1000</f>
+        <v>38321</v>
+      </c>
+      <c r="F4" s="65">
+        <f>GHG!F4 * 1000</f>
+        <v>1704495.3379226879</v>
+      </c>
+      <c r="G4" s="56"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="63">
+        <f>GHG!B5 * 1000</f>
+        <v>7903.3390978040006</v>
+      </c>
+      <c r="C5" s="64">
+        <f>GHG!C5 * 1000</f>
+        <v>6763.4080000000004</v>
+      </c>
+      <c r="D5" s="64">
+        <f>GHG!D5 * 1000</f>
+        <v>3874</v>
+      </c>
+      <c r="E5" s="64">
+        <f>GHG!E5 * 1000</f>
+        <v>2902.52</v>
+      </c>
+      <c r="F5" s="65">
+        <f>GHG!F5 * 1000</f>
+        <v>21443.267097804001</v>
+      </c>
+      <c r="G5" s="56"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="63">
+        <f>GHG!B6 * 1000</f>
+        <v>8440680.3619294614</v>
+      </c>
+      <c r="C6" s="64">
+        <f>GHG!C6 * 1000</f>
+        <v>3605315.0430000001</v>
+      </c>
+      <c r="D6" s="64">
+        <f>GHG!D6 * 1000</f>
+        <v>1137936.19829125</v>
+      </c>
+      <c r="E6" s="64">
+        <f>GHG!E6 * 1000</f>
+        <v>2830143.0000000005</v>
+      </c>
+      <c r="F6" s="65">
+        <f>GHG!F6 * 1000</f>
+        <v>16014074.603220711</v>
+      </c>
+      <c r="G6" s="56"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="63">
+        <v>94256.845479921001</v>
+      </c>
+      <c r="C7" s="64">
+        <v>534.73397999999997</v>
+      </c>
+      <c r="D7" s="64">
+        <v>3533.33012328</v>
+      </c>
+      <c r="E7" s="64">
+        <v>182.71</v>
+      </c>
+      <c r="F7" s="65">
+        <v>98507.619583200998</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="63">
+        <v>42846.268449704003</v>
+      </c>
+      <c r="C8" s="64">
+        <v>2085.8160600000001</v>
+      </c>
+      <c r="D8" s="64">
+        <v>1932.696238665</v>
+      </c>
+      <c r="E8" s="64">
+        <v>1662.99</v>
+      </c>
+      <c r="F8" s="65">
+        <v>48527.770748369003</v>
+      </c>
+      <c r="G8" s="56"/>
+    </row>
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="63">
+        <v>1548.1094865510001</v>
+      </c>
+      <c r="C9" s="64">
+        <v>929.76693999999998</v>
+      </c>
+      <c r="D9" s="64">
+        <v>120.18351857499999</v>
+      </c>
+      <c r="E9" s="64">
+        <v>102.75000000000001</v>
+      </c>
+      <c r="F9" s="65">
+        <v>2700.809945126</v>
+      </c>
+      <c r="G9" s="56"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="66">
+        <v>1246.1935030069999</v>
+      </c>
+      <c r="C10" s="67">
+        <v>114.93527</v>
+      </c>
+      <c r="D10" s="67">
+        <v>78.333718743999995</v>
+      </c>
+      <c r="E10" s="67">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="F10" s="68">
+        <v>1507.8624917509999</v>
+      </c>
+      <c r="G10" s="56"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G2:G6"/>
+    <mergeCell ref="G7:G10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BCBF7FB-3307-4FF3-9BFC-72AE6EAC5AEC}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="96" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2968,7 +3868,7 @@
       <c r="F2" s="13">
         <v>198.74997016</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="53" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2991,7 +3891,7 @@
       <c r="F3" s="13">
         <v>7.3924214342898988</v>
       </c>
-      <c r="G3" s="40"/>
+      <c r="G3" s="53"/>
     </row>
     <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
@@ -3012,7 +3912,7 @@
       <c r="F4" s="13">
         <v>206.1423915942899</v>
       </c>
-      <c r="G4" s="40"/>
+      <c r="G4" s="53"/>
     </row>
     <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
@@ -3039,12 +3939,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599D00AE-532C-4236-A29F-E6773C135A02}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3091,13 +3991,13 @@
       <c r="D2" s="4">
         <v>1.6238950000000001</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>28</v>
+      <c r="E2" s="8">
+        <v>0.2</v>
       </c>
       <c r="F2" s="13">
         <v>9.2238950000000006</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="47" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3120,7 +4020,7 @@
       <c r="F3" s="13">
         <v>52.633552000000002</v>
       </c>
-      <c r="G3" s="34"/>
+      <c r="G3" s="47"/>
     </row>
     <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="23" t="s">
@@ -3141,7 +4041,7 @@
       <c r="F4" s="13">
         <v>74.024124999999998</v>
       </c>
-      <c r="G4" s="34"/>
+      <c r="G4" s="47"/>
     </row>
     <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -3162,7 +4062,7 @@
       <c r="F5" s="13">
         <v>129.48417890000002</v>
       </c>
-      <c r="G5" s="34"/>
+      <c r="G5" s="47"/>
     </row>
     <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
@@ -3181,7 +4081,163 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E00972-0987-4121-BA5F-A181D5E41B6A}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="50.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="15"/>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="16"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="3">
+        <f>Water!B2 * 1000000</f>
+        <v>5400000</v>
+      </c>
+      <c r="C2" s="3">
+        <f>Water!C2 * 1000000</f>
+        <v>2100000</v>
+      </c>
+      <c r="D2" s="3">
+        <f>Water!D2 * 1000000</f>
+        <v>1623895</v>
+      </c>
+      <c r="E2" s="3">
+        <f>Water!E2 * 1000000</f>
+        <v>200000</v>
+      </c>
+      <c r="F2" s="3">
+        <f>Water!F2 * 1000000</f>
+        <v>9223895</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="3">
+        <f>Water!B3 * 1000000</f>
+        <v>26665239.999999996</v>
+      </c>
+      <c r="C3" s="3">
+        <f>Water!C3 * 1000000</f>
+        <v>113212</v>
+      </c>
+      <c r="D3" s="3">
+        <f>Water!D3 * 1000000</f>
+        <v>25854000</v>
+      </c>
+      <c r="E3" s="3">
+        <f>Water!E3 * 1000000</f>
+        <v>1100</v>
+      </c>
+      <c r="F3" s="3">
+        <f>Water!F3 * 1000000</f>
+        <v>52633552</v>
+      </c>
+      <c r="G3" s="47"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="3">
+        <f>Water!B4 * 1000000</f>
+        <v>49613560</v>
+      </c>
+      <c r="C4" s="3">
+        <f>Water!C4 * 1000000</f>
+        <v>24410565</v>
+      </c>
+      <c r="D4" s="3">
+        <f>Water!D4 * 1000000</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <f>Water!E4 * 1000000</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <f>Water!F4 * 1000000</f>
+        <v>74024125</v>
+      </c>
+      <c r="G4" s="47"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>129.48417890000002</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <v>129.48417890000002</v>
+      </c>
+      <c r="G5" s="47"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G2:G5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9FFD7F-7C5B-49EF-AEAC-F16A9FD511A8}">
   <dimension ref="A1:H8"/>
   <sheetViews>
@@ -3239,7 +4295,7 @@
       <c r="F2" s="13">
         <v>78599.760600000009</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="47" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3262,7 +4318,7 @@
       <c r="F3" s="13">
         <v>322488.61666</v>
       </c>
-      <c r="G3" s="34"/>
+      <c r="G3" s="47"/>
     </row>
     <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
@@ -3283,7 +4339,7 @@
       <c r="F4" s="13">
         <v>265507.54095000005</v>
       </c>
-      <c r="G4" s="34"/>
+      <c r="G4" s="47"/>
     </row>
     <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
@@ -3304,7 +4360,7 @@
       <c r="F5" s="13">
         <v>666595.91821000003</v>
       </c>
-      <c r="G5" s="34"/>
+      <c r="G5" s="47"/>
     </row>
     <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
@@ -3325,7 +4381,7 @@
       <c r="F6" s="13">
         <v>401088.37725999998</v>
       </c>
-      <c r="G6" s="34"/>
+      <c r="G6" s="47"/>
     </row>
     <row r="7" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
@@ -3352,7 +4408,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B326DB89-EB0C-40D8-9CBF-5F3D7B0A1993}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -3409,7 +4465,7 @@
       <c r="F2" s="13">
         <v>2</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="54" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3432,7 +4488,7 @@
       <c r="F3" s="13">
         <v>299</v>
       </c>
-      <c r="G3" s="41"/>
+      <c r="G3" s="54"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="23" t="s">
@@ -3453,7 +4509,7 @@
       <c r="F4" s="13">
         <v>99</v>
       </c>
-      <c r="G4" s="41"/>
+      <c r="G4" s="54"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -3474,7 +4530,7 @@
       <c r="F5" s="13">
         <v>861</v>
       </c>
-      <c r="G5" s="41"/>
+      <c r="G5" s="54"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="23" t="s">
@@ -3495,7 +4551,7 @@
       <c r="F6" s="13">
         <v>496</v>
       </c>
-      <c r="G6" s="41"/>
+      <c r="G6" s="54"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
@@ -3520,402 +4576,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C4FF68-BC2E-4B44-9D83-60450A12F19E}">
-  <dimension ref="A1:H12"/>
-  <sheetViews>
-    <sheetView zoomScale="110" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="45.81640625" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="15"/>
-      <c r="B1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="16"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="3">
-        <v>445.21</v>
-      </c>
-      <c r="C2" s="4">
-        <v>64.026368000000005</v>
-      </c>
-      <c r="D2" s="4">
-        <v>80.385821050000004</v>
-      </c>
-      <c r="E2" s="4">
-        <v>98.66</v>
-      </c>
-      <c r="F2" s="13">
-        <v>688.28218905000006</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="7">
-        <f>989+200</f>
-        <v>1189</v>
-      </c>
-      <c r="C3" s="8">
-        <v>85</v>
-      </c>
-      <c r="D3" s="8">
-        <v>248</v>
-      </c>
-      <c r="E3" s="12">
-        <v>216</v>
-      </c>
-      <c r="F3" s="27">
-        <f>SUM(B3:E3)</f>
-        <v>1738</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="3">
-        <f>3+1.5</f>
-        <v>4.5</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E4" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="F4" s="27">
-        <f t="shared" ref="F4:F9" si="0">SUM(B4:E4)</f>
-        <v>5.4</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="3">
-        <f>5.6+1.1</f>
-        <v>6.6999999999999993</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="13">
-        <v>1.9</v>
-      </c>
-      <c r="F5" s="27">
-        <f t="shared" si="0"/>
-        <v>10.1</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="3">
-        <f>10.3+1.8</f>
-        <v>12.100000000000001</v>
-      </c>
-      <c r="C6" s="4">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D6" s="4">
-        <v>3.2</v>
-      </c>
-      <c r="E6" s="13">
-        <v>7.1</v>
-      </c>
-      <c r="F6" s="27">
-        <f t="shared" si="0"/>
-        <v>24.6</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4">
-        <v>3</v>
-      </c>
-      <c r="E7" s="13">
-        <v>3</v>
-      </c>
-      <c r="F7" s="27">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G7" s="35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="3">
-        <v>7</v>
-      </c>
-      <c r="C8" s="4">
-        <v>2</v>
-      </c>
-      <c r="D8" s="4">
-        <v>6</v>
-      </c>
-      <c r="E8" s="13">
-        <v>5</v>
-      </c>
-      <c r="F8" s="27">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="G8" s="36"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="5">
-        <v>3</v>
-      </c>
-      <c r="C9" s="6">
-        <v>1</v>
-      </c>
-      <c r="D9" s="6">
-        <v>5</v>
-      </c>
-      <c r="E9" s="14">
-        <v>4</v>
-      </c>
-      <c r="F9" s="28">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="G9" s="37"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="G7:G9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD8AEB7-D2E8-4525-A681-2676EB3834C0}">
-  <dimension ref="A1:E8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="30.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="44" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="46">
-        <f xml:space="preserve"> 20000 / [1]GHG!A6 + 2000 / SUM( [1]GHG!A8:A12)</f>
-        <v>2.3823084554870104</v>
-      </c>
-      <c r="C2" s="46">
-        <f xml:space="preserve"> 20000 / [1]GHG!B6 + 2000 / SUM( [1]GHG!B8:B12)</f>
-        <v>6.0596389501013492</v>
-      </c>
-      <c r="D2" s="46">
-        <f xml:space="preserve"> 20000 / [1]GHG!C6 + 2000 / SUM( [1]GHG!C8:C12)</f>
-        <v>17.894930089120145</v>
-      </c>
-      <c r="E2" s="46">
-        <f xml:space="preserve"> 20000 / [1]GHG!D6 + 2000 / SUM( [1]GHG!D8:D12)</f>
-        <v>7.719658610227814</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="48">
-        <f>333 / [1]Energy!A4</f>
-        <v>3.8305302805152781</v>
-      </c>
-      <c r="C3" s="48">
-        <f>333 / [1]Energy!B4</f>
-        <v>5.5438751267570021</v>
-      </c>
-      <c r="D3" s="48">
-        <f>333 / [1]Energy!C4</f>
-        <v>19.753267851317634</v>
-      </c>
-      <c r="E3" s="48">
-        <f>333 / [1]Energy!D4</f>
-        <v>7.8751330258957086</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="48">
-        <f>1 / SUM([1]Water!A2:A3) + [1]Water!A4 / 1000 + 5 / ([1]Water!A5 + 1)</f>
-        <v>5.0807999786888978</v>
-      </c>
-      <c r="C4" s="48">
-        <f>1 / SUM([1]Water!B2:B3) + [1]Water!B4 / 1000 + 5 / ([1]Water!B5 + 1)</f>
-        <v>5.4762425630191682</v>
-      </c>
-      <c r="D4" s="48">
-        <f>1 / SUM([1]Water!C2:C3) + [1]Water!C4 / 1000 + 5 / ([1]Water!C5 + 1)</f>
-        <v>7.4711711437762368E-2</v>
-      </c>
-      <c r="E4" s="48">
-        <f>1 / SUM([1]Water!D2:D3) + [1]Water!D4 / 1000 + 5 / ([1]Water!D5 + 1)</f>
-        <v>914.09090909090901</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="49"/>
-    </row>
-    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="50" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="52"/>
-    </row>
-    <row r="7" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="54">
-        <f>SUM(B2:B6)</f>
-        <v>11.293638714691186</v>
-      </c>
-      <c r="C7" s="54">
-        <f t="shared" ref="C7:E7" si="0">SUM(C2:C6)</f>
-        <v>17.07975663987752</v>
-      </c>
-      <c r="D7" s="54">
-        <f t="shared" si="0"/>
-        <v>37.722909651875547</v>
-      </c>
-      <c r="E7" s="54">
-        <f t="shared" si="0"/>
-        <v>929.68570072703255</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
made sustainability scores sheet
</commit_message>
<xml_diff>
--- a/Data Sets (Excels)/Data (1) (3).xlsx
+++ b/Data Sets (Excels)/Data (1) (3).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofh-my.sharepoint.com/personal/jmfalou_cougarnet_uh_edu/Documents/~Computer Science/z. Hackathon Projects/HalfStackDevs_CodeRedGenesis/Data Sets (Excels)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{B116884D-3ADB-43C2-93BC-1D797EACA0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5111178C-C32A-405B-84E6-699AF57D58E3}"/>
+  <xr:revisionPtr revIDLastSave="224" documentId="8_{B116884D-3ADB-43C2-93BC-1D797EACA0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{943D6497-6BCF-4B73-B9E2-25E97ADDCFCE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="2" activeTab="3" xr2:uid="{01528FDC-71FA-430E-A617-D3435C6CD15B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="4" activeTab="10" xr2:uid="{01528FDC-71FA-430E-A617-D3435C6CD15B}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <sheet name="Production and Facility Info" sheetId="7" r:id="rId10"/>
     <sheet name="Sustainability Scores" sheetId="9" r:id="rId11"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId12"/>
-  </externalReferences>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -49,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="75">
   <si>
     <t>U.S.A.</t>
   </si>
@@ -271,6 +268,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tonnes </t>
+  </si>
+  <si>
+    <t>MEAN</t>
   </si>
 </sst>
 </file>
@@ -282,7 +282,7 @@
     <numFmt numFmtId="164" formatCode="#,###"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +358,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -379,7 +401,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="53">
+  <borders count="56">
     <border>
       <left/>
       <right/>
@@ -839,55 +861,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
         <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color auto="1"/>
       </left>
       <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
         <color auto="1"/>
       </right>
       <top style="thin">
@@ -1105,6 +1097,77 @@
       <bottom style="thick">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1116,7 +1179,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
@@ -1165,15 +1228,21 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="39" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="40" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="41" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1201,21 +1270,19 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="40" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="38" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="41" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="42" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="43" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{6E9C2E63-9F6E-43C0-BFCD-2DC1E9F19C6C}"/>
@@ -1236,193 +1303,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="ALL"/>
-      <sheetName val="Sustainability Scores"/>
-      <sheetName val="GHG"/>
-      <sheetName val="Energy"/>
-      <sheetName val="Water"/>
-      <sheetName val="Waste"/>
-      <sheetName val="Spills"/>
-      <sheetName val="Production and Facility Info"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2">
-        <row r="6">
-          <cell r="A6">
-            <v>8440.6803619294606</v>
-          </cell>
-          <cell r="B6">
-            <v>3605.3150430000001</v>
-          </cell>
-          <cell r="C6">
-            <v>1137.9361982912501</v>
-          </cell>
-          <cell r="D6">
-            <v>2830.1430000000005</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>15972.450569727</v>
-          </cell>
-          <cell r="B8">
-            <v>238.91200000000001</v>
-          </cell>
-          <cell r="C8">
-            <v>600.09470903299996</v>
-          </cell>
-          <cell r="D8">
-            <v>1046.51</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>94256.845479921001</v>
-          </cell>
-          <cell r="B9">
-            <v>534.73397999999997</v>
-          </cell>
-          <cell r="C9">
-            <v>3533.33012328</v>
-          </cell>
-          <cell r="D9">
-            <v>182.71</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>42846.268449704003</v>
-          </cell>
-          <cell r="B10">
-            <v>2085.8160600000001</v>
-          </cell>
-          <cell r="C10">
-            <v>1932.696238665</v>
-          </cell>
-          <cell r="D10">
-            <v>1662.99</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>1548.1094865510001</v>
-          </cell>
-          <cell r="B11">
-            <v>929.76693999999998</v>
-          </cell>
-          <cell r="C11">
-            <v>120.18351857499999</v>
-          </cell>
-          <cell r="D11">
-            <v>102.75000000000001</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>1246.1935030069999</v>
-          </cell>
-          <cell r="B12">
-            <v>114.93527</v>
-          </cell>
-          <cell r="C12">
-            <v>78.333718743999995</v>
-          </cell>
-          <cell r="D12">
-            <v>68.400000000000006</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3">
-        <row r="4">
-          <cell r="A4">
-            <v>86.933133434257897</v>
-          </cell>
-          <cell r="B4">
-            <v>60.066288000032003</v>
-          </cell>
-          <cell r="C4">
-            <v>16.857970160000001</v>
-          </cell>
-          <cell r="D4">
-            <v>42.284999999999997</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4">
-        <row r="2">
-          <cell r="A2">
-            <v>5.4</v>
-          </cell>
-          <cell r="B2">
-            <v>2.1</v>
-          </cell>
-          <cell r="C2">
-            <v>1.6238950000000001</v>
-          </cell>
-          <cell r="D2" t="str">
-            <v>&lt;0.2</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>26.665239999999997</v>
-          </cell>
-          <cell r="B3">
-            <v>0.11321200000000001</v>
-          </cell>
-          <cell r="C3">
-            <v>25.853999999999999</v>
-          </cell>
-          <cell r="D3">
-            <v>1.1000000000000001E-3</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>49.61356</v>
-          </cell>
-          <cell r="B4">
-            <v>24.410564999999998</v>
-          </cell>
-          <cell r="C4">
-            <v>0</v>
-          </cell>
-          <cell r="D4">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>0</v>
-          </cell>
-          <cell r="B5">
-            <v>0</v>
-          </cell>
-          <cell r="C5">
-            <v>129.48417890000002</v>
-          </cell>
-          <cell r="D5">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1790,7 +1670,7 @@
       <c r="F2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="G2" s="57" t="s">
         <v>8</v>
       </c>
       <c r="M2" s="8">
@@ -1819,7 +1699,7 @@
       <c r="F3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="58"/>
       <c r="M3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1846,7 +1726,7 @@
       <c r="F4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="58"/>
       <c r="M4" s="4">
         <v>28.360250000000001</v>
       </c>
@@ -1873,7 +1753,7 @@
       <c r="F5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="52"/>
+      <c r="G5" s="58"/>
       <c r="M5" s="4">
         <v>1.7284000000000002</v>
       </c>
@@ -1900,7 +1780,7 @@
       <c r="F6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="52"/>
+      <c r="G6" s="58"/>
       <c r="M6" s="4">
         <v>2133.6398300000005</v>
       </c>
@@ -1985,7 +1865,7 @@
       <c r="F9" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="58" t="s">
         <v>20</v>
       </c>
       <c r="M9" s="4">
@@ -2014,7 +1894,7 @@
       <c r="F10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="52"/>
+      <c r="G10" s="58"/>
       <c r="M10" s="4">
         <v>1193.19</v>
       </c>
@@ -2041,7 +1921,7 @@
       <c r="F11" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="52"/>
+      <c r="G11" s="58"/>
       <c r="M11" s="4">
         <v>14.73</v>
       </c>
@@ -2068,7 +1948,7 @@
       <c r="F12" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="52"/>
+      <c r="G12" s="58"/>
       <c r="M12" s="4">
         <v>52</v>
       </c>
@@ -2095,7 +1975,7 @@
       <c r="F13" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="53" t="s">
+      <c r="G13" s="59" t="s">
         <v>25</v>
       </c>
       <c r="M13" s="4">
@@ -2124,7 +2004,7 @@
       <c r="F14" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="53"/>
+      <c r="G14" s="59"/>
       <c r="M14" s="4">
         <v>0</v>
       </c>
@@ -2151,7 +2031,7 @@
       <c r="F15" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="53"/>
+      <c r="G15" s="59"/>
       <c r="M15" s="4">
         <v>38.119999999999997</v>
       </c>
@@ -2178,7 +2058,7 @@
       <c r="F16" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="47" t="s">
+      <c r="G16" s="53" t="s">
         <v>30</v>
       </c>
       <c r="M16" s="4" t="s">
@@ -2207,7 +2087,7 @@
       <c r="F17" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="47"/>
+      <c r="G17" s="53"/>
       <c r="M17" s="4">
         <v>0</v>
       </c>
@@ -2234,7 +2114,7 @@
       <c r="F18" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="47"/>
+      <c r="G18" s="53"/>
       <c r="M18" s="4">
         <v>0</v>
       </c>
@@ -2261,7 +2141,7 @@
       <c r="F19" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="47"/>
+      <c r="G19" s="53"/>
       <c r="M19" s="4">
         <v>0</v>
       </c>
@@ -2288,7 +2168,7 @@
       <c r="F20" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="54" t="s">
+      <c r="G20" s="60" t="s">
         <v>36</v>
       </c>
       <c r="M20" s="4">
@@ -2317,7 +2197,7 @@
       <c r="F21" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="54"/>
+      <c r="G21" s="60"/>
       <c r="M21" s="4">
         <v>0</v>
       </c>
@@ -2344,7 +2224,7 @@
       <c r="F22" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="54"/>
+      <c r="G22" s="60"/>
       <c r="M22" s="4">
         <v>0</v>
       </c>
@@ -2371,7 +2251,7 @@
       <c r="F23" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="54"/>
+      <c r="G23" s="60"/>
       <c r="M23" s="4">
         <v>0</v>
       </c>
@@ -2398,7 +2278,7 @@
       <c r="F24" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="54"/>
+      <c r="G24" s="60"/>
       <c r="M24" s="4">
         <v>0</v>
       </c>
@@ -2425,7 +2305,7 @@
       <c r="F25" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="G25" s="47" t="s">
+      <c r="G25" s="53" t="s">
         <v>42</v>
       </c>
       <c r="M25" s="4">
@@ -2454,7 +2334,7 @@
       <c r="F26" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="47"/>
+      <c r="G26" s="53"/>
       <c r="M26" s="4">
         <v>144.52000000000001</v>
       </c>
@@ -2481,7 +2361,7 @@
       <c r="F27" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G27" s="47"/>
+      <c r="G27" s="53"/>
       <c r="M27" s="4">
         <v>518.64</v>
       </c>
@@ -2508,7 +2388,7 @@
       <c r="F28" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G28" s="47"/>
+      <c r="G28" s="53"/>
       <c r="M28" s="4">
         <v>667.57999999999993</v>
       </c>
@@ -2535,7 +2415,7 @@
       <c r="F29" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G29" s="47"/>
+      <c r="G29" s="53"/>
       <c r="M29" s="4">
         <v>148.94</v>
       </c>
@@ -2692,7 +2572,7 @@
       <c r="F35" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="G35" s="48" t="s">
+      <c r="G35" s="54" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2716,7 +2596,7 @@
       <c r="F36" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G36" s="49"/>
+      <c r="G36" s="55"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="5">
@@ -2738,7 +2618,7 @@
       <c r="F37" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="G37" s="50"/>
+      <c r="G37" s="56"/>
     </row>
     <row r="38" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="H38" s="1"/>
@@ -2784,7 +2664,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView zoomScale="110" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2960,7 +2840,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G7" s="48" t="s">
+      <c r="G7" s="54" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2984,7 +2864,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G8" s="49"/>
+      <c r="G8" s="55"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="24" t="s">
@@ -3006,7 +2886,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="G9" s="50"/>
+      <c r="G9" s="56"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H10" s="1"/>
@@ -3040,10 +2920,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD8AEB7-D2E8-4525-A681-2676EB3834C0}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3055,7 +2935,7 @@
     <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="34" t="s">
         <v>0</v>
       </c>
@@ -3068,110 +2948,158 @@
       <c r="E1" s="36" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="16" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="F1" s="67" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="38">
-        <f xml:space="preserve"> 20000 / [1]GHG!A6 + 2000 / SUM( [1]GHG!A8:A12)</f>
-        <v>2.3823084554870104</v>
-      </c>
-      <c r="C2" s="38">
-        <f xml:space="preserve"> 20000 / [1]GHG!B6 + 2000 / SUM( [1]GHG!B8:B12)</f>
-        <v>6.0596389501013492</v>
-      </c>
-      <c r="D2" s="38">
-        <f xml:space="preserve"> 20000 / [1]GHG!C6 + 2000 / SUM( [1]GHG!C8:C12)</f>
-        <v>17.894930089120145</v>
-      </c>
-      <c r="E2" s="38">
-        <f xml:space="preserve"> 20000 / [1]GHG!D6 + 2000 / SUM( [1]GHG!D8:D12)</f>
-        <v>7.719658610227814</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="39" t="s">
+      <c r="B2" s="63">
+        <f xml:space="preserve"> 20 - SUM('GHG (Uniform Units)'!B2:B10) /'Production and Facility Info'!B6 / 160000</f>
+        <v>11.20802781984602</v>
+      </c>
+      <c r="C2" s="63">
+        <f xml:space="preserve"> 20 - SUM('GHG (Uniform Units)'!C2:C10) /'Production and Facility Info'!C6 / 160000</f>
+        <v>-0.49515721093749576</v>
+      </c>
+      <c r="D2" s="63">
+        <f xml:space="preserve"> 20 - SUM('GHG (Uniform Units)'!D2:D10) /'Production and Facility Info'!D6 / 160000</f>
+        <v>15.543873163707492</v>
+      </c>
+      <c r="E2" s="63">
+        <f xml:space="preserve"> 20 - SUM('GHG (Uniform Units)'!E2:E10) /'Production and Facility Info'!E6 / 160000</f>
+        <v>15.014786223591548</v>
+      </c>
+      <c r="F2" s="69">
+        <f>AVERAGE(B2:E2)</f>
+        <v>10.31788249905189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="40">
-        <f>333 / [1]Energy!A4</f>
-        <v>3.8305302805152781</v>
-      </c>
-      <c r="C3" s="40">
-        <f>333 / [1]Energy!B4</f>
-        <v>5.5438751267570021</v>
-      </c>
-      <c r="D3" s="40">
-        <f>333 / [1]Energy!C4</f>
-        <v>19.753267851317634</v>
-      </c>
-      <c r="E3" s="40">
-        <f>333 / [1]Energy!D4</f>
-        <v>7.8751330258957086</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="39" t="s">
+      <c r="B3" s="64">
+        <f>20 -  Energy!B4 /'Production and Facility Info'!B6 / 1</f>
+        <v>12.815443517829927</v>
+      </c>
+      <c r="C3" s="64">
+        <v>0</v>
+      </c>
+      <c r="D3" s="64">
+        <f>20 -  Energy!D4 /'Production and Facility Info'!D6 / 1</f>
+        <v>14.731884324999999</v>
+      </c>
+      <c r="E3" s="64">
+        <f>20 -  Energy!E4 /'Production and Facility Info'!E6 / 1</f>
+        <v>14.044366197183098</v>
+      </c>
+      <c r="F3" s="70">
+        <f t="shared" ref="F3:F7" si="0">AVERAGE(B3:E3)</f>
+        <v>10.397923510003256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="40">
-        <f>1 / SUM([1]Water!A2:A3) + [1]Water!A4 / 1000 + 5 / ([1]Water!A5 + 1)</f>
-        <v>5.0807999786888978</v>
-      </c>
-      <c r="C4" s="40">
-        <f>1 / SUM([1]Water!B2:B3) + [1]Water!B4 / 1000 + 5 / ([1]Water!B5 + 1)</f>
-        <v>5.4762425630191682</v>
-      </c>
-      <c r="D4" s="40">
-        <f>1 / SUM([1]Water!C2:C3) + [1]Water!C4 / 1000 + 5 / ([1]Water!C5 + 1)</f>
-        <v>7.4711711437762368E-2</v>
-      </c>
-      <c r="E4" s="40">
-        <f>1 / SUM([1]Water!D2:D3) + [1]Water!D4 / 1000 + 5 / ([1]Water!D5 + 1)</f>
-        <v>914.09090909090901</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="39" t="s">
+      <c r="B4" s="64">
+        <f xml:space="preserve"> 20 - (SUM('Water (Uniform Units)'!B2:B3) + 1000000 * 'Water (Uniform Units)'!B5) / 'Production and Facility Info'!B6 / 200000</f>
+        <v>6.7499008264462841</v>
+      </c>
+      <c r="C4" s="64">
+        <f xml:space="preserve"> 20 - (SUM('Water (Uniform Units)'!C2:C3) + 1000000 * 'Water (Uniform Units)'!C5) / 'Production and Facility Info'!C6 / 200000</f>
+        <v>14.969972727272728</v>
+      </c>
+      <c r="D4" s="64">
+        <v>0</v>
+      </c>
+      <c r="E4" s="64">
+        <f xml:space="preserve"> 20 - (SUM('Water (Uniform Units)'!E2:E3) + 1000000 * 'Water (Uniform Units)'!E5) / 'Production and Facility Info'!E6 / 200000</f>
+        <v>19.858380281690142</v>
+      </c>
+      <c r="F4" s="70">
+        <f t="shared" si="0"/>
+        <v>10.394563458852289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="41"/>
-    </row>
-    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="42" t="s">
+      <c r="B5" s="64">
+        <v>0</v>
+      </c>
+      <c r="C5" s="64">
+        <f>20 - (Waste!C5-Waste!C6)/'Production and Facility Info'!C6 / 250</f>
+        <v>10.343636363636364</v>
+      </c>
+      <c r="D5" s="64">
+        <f>20 - (Waste!D5-Waste!D6)/'Production and Facility Info'!D6 / 250</f>
+        <v>11.038861312500002</v>
+      </c>
+      <c r="E5" s="64">
+        <f>20 - (Waste!E5-Waste!E6)/'Production and Facility Info'!E6 / 250</f>
+        <v>19.693256338028171</v>
+      </c>
+      <c r="F5" s="70">
+        <f t="shared" si="0"/>
+        <v>10.268938503541134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="44"/>
-    </row>
-    <row r="7" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="45" t="s">
+      <c r="B6" s="65">
+        <f>20 - (Spills!B3+Spills!B5-Spills!B6)/'Production and Facility Info'!B6 / 2.5</f>
+        <v>1.6859504132231429</v>
+      </c>
+      <c r="C6" s="65">
+        <f>20 - (Spills!C3+Spills!C5-Spills!C6)/'Production and Facility Info'!C6 / 2.5</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="65">
+        <f>20 - (Spills!D3+Spills!D5-Spills!D6)/'Production and Facility Info'!D6 / 2.5</f>
+        <v>20</v>
+      </c>
+      <c r="E6" s="65">
+        <f>20 - (Spills!E3+Spills!E5-Spills!E6)/'Production and Facility Info'!E6 / 2.5</f>
+        <v>20</v>
+      </c>
+      <c r="F6" s="71">
+        <f t="shared" si="0"/>
+        <v>10.421487603305785</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="66">
         <f>SUM(B2:B6)</f>
-        <v>11.293638714691186</v>
-      </c>
-      <c r="C7" s="46">
-        <f t="shared" ref="C7:E7" si="0">SUM(C2:C6)</f>
-        <v>17.07975663987752</v>
-      </c>
-      <c r="D7" s="46">
-        <f t="shared" si="0"/>
-        <v>37.722909651875547</v>
-      </c>
-      <c r="E7" s="46">
-        <f t="shared" si="0"/>
-        <v>929.68570072703255</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+        <v>32.459322577345375</v>
+      </c>
+      <c r="C7" s="66">
+        <f t="shared" ref="C7:E7" si="1">SUM(C2:C6)</f>
+        <v>24.818451879971597</v>
+      </c>
+      <c r="D7" s="66">
+        <f t="shared" si="1"/>
+        <v>61.314618801207494</v>
+      </c>
+      <c r="E7" s="68">
+        <f t="shared" si="1"/>
+        <v>88.610789040492961</v>
+      </c>
+      <c r="F7" s="72">
+        <f>AVERAGE(B7:E7)</f>
+        <v>51.80079557475436</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3283,7 +3211,7 @@
       <c r="F2" s="12">
         <v>13228.247138200219</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="G2" s="57" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3306,7 +3234,7 @@
       <c r="F3" s="13">
         <v>1059.88886</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="58"/>
     </row>
     <row r="4" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
@@ -3327,7 +3255,7 @@
       <c r="F4" s="13">
         <v>1704.4953379226879</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="58"/>
     </row>
     <row r="5" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
@@ -3348,7 +3276,7 @@
       <c r="F5" s="13">
         <v>21.443267097804</v>
       </c>
-      <c r="G5" s="52"/>
+      <c r="G5" s="58"/>
     </row>
     <row r="6" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
@@ -3369,7 +3297,7 @@
       <c r="F6" s="13">
         <v>16014.07460322071</v>
       </c>
-      <c r="G6" s="52"/>
+      <c r="G6" s="58"/>
     </row>
     <row r="7" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
@@ -3436,7 +3364,7 @@
       <c r="F9" s="13">
         <v>98507.619583200998</v>
       </c>
-      <c r="G9" s="52" t="s">
+      <c r="G9" s="58" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3459,7 +3387,7 @@
       <c r="F10" s="13">
         <v>48527.770748369003</v>
       </c>
-      <c r="G10" s="52"/>
+      <c r="G10" s="58"/>
     </row>
     <row r="11" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
@@ -3480,7 +3408,7 @@
       <c r="F11" s="13">
         <v>2700.809945126</v>
       </c>
-      <c r="G11" s="52"/>
+      <c r="G11" s="58"/>
     </row>
     <row r="12" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
@@ -3501,7 +3429,7 @@
       <c r="F12" s="13">
         <v>1507.8624917509999</v>
       </c>
-      <c r="G12" s="52"/>
+      <c r="G12" s="58"/>
     </row>
     <row r="13" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
@@ -3533,8 +3461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B11A20-252D-4AB9-80BE-AA57F15F88DC}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3549,19 +3477,19 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="15"/>
-      <c r="B1" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="58" t="s">
+      <c r="B1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="43" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="16"/>
@@ -3570,27 +3498,27 @@
       <c r="A2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="60">
+      <c r="B2" s="44">
         <f>GHG!B2 * 1000</f>
         <v>6129143.1650302196</v>
       </c>
-      <c r="C2" s="61">
+      <c r="C2" s="45">
         <f>GHG!C2 * 1000</f>
         <v>3216656.88</v>
       </c>
-      <c r="D2" s="61">
+      <c r="D2" s="45">
         <f>GHG!D2 * 1000</f>
         <v>1093527.61317</v>
       </c>
-      <c r="E2" s="61">
+      <c r="E2" s="45">
         <f>GHG!E2 * 1000</f>
         <v>2788919.4800000004</v>
       </c>
-      <c r="F2" s="62">
+      <c r="F2" s="46">
         <f>GHG!F2 * 1000</f>
         <v>13228247.138200218</v>
       </c>
-      <c r="G2" s="55" t="s">
+      <c r="G2" s="61" t="s">
         <v>68</v>
       </c>
     </row>
@@ -3598,126 +3526,126 @@
       <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="63">
+      <c r="B3" s="47">
         <f>GHG!B3 * 1000</f>
         <v>710732.03</v>
       </c>
-      <c r="C3" s="64">
+      <c r="C3" s="48">
         <f>GHG!C3 * 1000</f>
         <v>335608.83</v>
       </c>
-      <c r="D3" s="64">
+      <c r="D3" s="48">
         <f>GHG!D3 * 1000</f>
         <v>13548</v>
       </c>
-      <c r="E3" s="64">
+      <c r="E3" s="48">
         <f>GHG!E3 * 1000</f>
         <v>900</v>
       </c>
-      <c r="F3" s="65">
+      <c r="F3" s="49">
         <f>GHG!F3 * 1000</f>
         <v>1059888.8600000001</v>
       </c>
-      <c r="G3" s="56"/>
+      <c r="G3" s="62"/>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="63">
+      <c r="B4" s="47">
         <f>GHG!B4 * 1000</f>
         <v>1592901.827801438</v>
       </c>
-      <c r="C4" s="64">
+      <c r="C4" s="48">
         <f>GHG!C4 * 1000</f>
         <v>46285.925000000003</v>
       </c>
-      <c r="D4" s="64">
+      <c r="D4" s="48">
         <f>GHG!D4 * 1000</f>
         <v>26986.585121249998</v>
       </c>
-      <c r="E4" s="64">
+      <c r="E4" s="48">
         <f>GHG!E4 * 1000</f>
         <v>38321</v>
       </c>
-      <c r="F4" s="65">
+      <c r="F4" s="49">
         <f>GHG!F4 * 1000</f>
         <v>1704495.3379226879</v>
       </c>
-      <c r="G4" s="56"/>
+      <c r="G4" s="62"/>
     </row>
     <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="63">
+      <c r="B5" s="47">
         <f>GHG!B5 * 1000</f>
         <v>7903.3390978040006</v>
       </c>
-      <c r="C5" s="64">
+      <c r="C5" s="48">
         <f>GHG!C5 * 1000</f>
         <v>6763.4080000000004</v>
       </c>
-      <c r="D5" s="64">
+      <c r="D5" s="48">
         <f>GHG!D5 * 1000</f>
         <v>3874</v>
       </c>
-      <c r="E5" s="64">
+      <c r="E5" s="48">
         <f>GHG!E5 * 1000</f>
         <v>2902.52</v>
       </c>
-      <c r="F5" s="65">
+      <c r="F5" s="49">
         <f>GHG!F5 * 1000</f>
         <v>21443.267097804001</v>
       </c>
-      <c r="G5" s="56"/>
+      <c r="G5" s="62"/>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="63">
+      <c r="B6" s="47">
         <f>GHG!B6 * 1000</f>
         <v>8440680.3619294614</v>
       </c>
-      <c r="C6" s="64">
+      <c r="C6" s="48">
         <f>GHG!C6 * 1000</f>
         <v>3605315.0430000001</v>
       </c>
-      <c r="D6" s="64">
+      <c r="D6" s="48">
         <f>GHG!D6 * 1000</f>
         <v>1137936.19829125</v>
       </c>
-      <c r="E6" s="64">
+      <c r="E6" s="48">
         <f>GHG!E6 * 1000</f>
         <v>2830143.0000000005</v>
       </c>
-      <c r="F6" s="65">
+      <c r="F6" s="49">
         <f>GHG!F6 * 1000</f>
         <v>16014074.603220711</v>
       </c>
-      <c r="G6" s="56"/>
+      <c r="G6" s="62"/>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="63">
+      <c r="B7" s="47">
         <v>94256.845479921001</v>
       </c>
-      <c r="C7" s="64">
+      <c r="C7" s="48">
         <v>534.73397999999997</v>
       </c>
-      <c r="D7" s="64">
+      <c r="D7" s="48">
         <v>3533.33012328</v>
       </c>
-      <c r="E7" s="64">
+      <c r="E7" s="48">
         <v>182.71</v>
       </c>
-      <c r="F7" s="65">
+      <c r="F7" s="49">
         <v>98507.619583200998</v>
       </c>
-      <c r="G7" s="56" t="s">
+      <c r="G7" s="62" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3725,64 +3653,64 @@
       <c r="A8" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="63">
+      <c r="B8" s="47">
         <v>42846.268449704003</v>
       </c>
-      <c r="C8" s="64">
+      <c r="C8" s="48">
         <v>2085.8160600000001</v>
       </c>
-      <c r="D8" s="64">
+      <c r="D8" s="48">
         <v>1932.696238665</v>
       </c>
-      <c r="E8" s="64">
+      <c r="E8" s="48">
         <v>1662.99</v>
       </c>
-      <c r="F8" s="65">
+      <c r="F8" s="49">
         <v>48527.770748369003</v>
       </c>
-      <c r="G8" s="56"/>
+      <c r="G8" s="62"/>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="63">
+      <c r="B9" s="47">
         <v>1548.1094865510001</v>
       </c>
-      <c r="C9" s="64">
+      <c r="C9" s="48">
         <v>929.76693999999998</v>
       </c>
-      <c r="D9" s="64">
+      <c r="D9" s="48">
         <v>120.18351857499999</v>
       </c>
-      <c r="E9" s="64">
+      <c r="E9" s="48">
         <v>102.75000000000001</v>
       </c>
-      <c r="F9" s="65">
+      <c r="F9" s="49">
         <v>2700.809945126</v>
       </c>
-      <c r="G9" s="56"/>
+      <c r="G9" s="62"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="66">
+      <c r="B10" s="50">
         <v>1246.1935030069999</v>
       </c>
-      <c r="C10" s="67">
+      <c r="C10" s="51">
         <v>114.93527</v>
       </c>
-      <c r="D10" s="67">
+      <c r="D10" s="51">
         <v>78.333718743999995</v>
       </c>
-      <c r="E10" s="67">
+      <c r="E10" s="51">
         <v>68.400000000000006</v>
       </c>
-      <c r="F10" s="68">
+      <c r="F10" s="52">
         <v>1507.8624917509999</v>
       </c>
-      <c r="G10" s="56"/>
+      <c r="G10" s="62"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
@@ -3868,7 +3796,7 @@
       <c r="F2" s="13">
         <v>198.74997016</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="59" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3891,7 +3819,7 @@
       <c r="F3" s="13">
         <v>7.3924214342898988</v>
       </c>
-      <c r="G3" s="53"/>
+      <c r="G3" s="59"/>
     </row>
     <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
@@ -3912,7 +3840,7 @@
       <c r="F4" s="13">
         <v>206.1423915942899</v>
       </c>
-      <c r="G4" s="53"/>
+      <c r="G4" s="59"/>
     </row>
     <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
@@ -3997,7 +3925,7 @@
       <c r="F2" s="13">
         <v>9.2238950000000006</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="53" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4020,7 +3948,7 @@
       <c r="F3" s="13">
         <v>52.633552000000002</v>
       </c>
-      <c r="G3" s="47"/>
+      <c r="G3" s="53"/>
     </row>
     <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="23" t="s">
@@ -4041,7 +3969,7 @@
       <c r="F4" s="13">
         <v>74.024124999999998</v>
       </c>
-      <c r="G4" s="47"/>
+      <c r="G4" s="53"/>
     </row>
     <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -4062,7 +3990,7 @@
       <c r="F5" s="13">
         <v>129.48417890000002</v>
       </c>
-      <c r="G5" s="47"/>
+      <c r="G5" s="53"/>
     </row>
     <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
@@ -4086,7 +4014,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4143,7 +4071,7 @@
         <f>Water!F2 * 1000000</f>
         <v>9223895</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="53" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4171,7 +4099,7 @@
         <f>Water!F3 * 1000000</f>
         <v>52633552</v>
       </c>
-      <c r="G3" s="47"/>
+      <c r="G3" s="53"/>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="23" t="s">
@@ -4197,7 +4125,7 @@
         <f>Water!F4 * 1000000</f>
         <v>74024125</v>
       </c>
-      <c r="G4" s="47"/>
+      <c r="G4" s="53"/>
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="23" t="s">
@@ -4218,7 +4146,7 @@
       <c r="F5" s="13">
         <v>129.48417890000002</v>
       </c>
-      <c r="G5" s="47"/>
+      <c r="G5" s="53"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
@@ -4295,7 +4223,7 @@
       <c r="F2" s="13">
         <v>78599.760600000009</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="53" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4318,7 +4246,7 @@
       <c r="F3" s="13">
         <v>322488.61666</v>
       </c>
-      <c r="G3" s="47"/>
+      <c r="G3" s="53"/>
     </row>
     <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
@@ -4339,7 +4267,7 @@
       <c r="F4" s="13">
         <v>265507.54095000005</v>
       </c>
-      <c r="G4" s="47"/>
+      <c r="G4" s="53"/>
     </row>
     <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
@@ -4360,7 +4288,7 @@
       <c r="F5" s="13">
         <v>666595.91821000003</v>
       </c>
-      <c r="G5" s="47"/>
+      <c r="G5" s="53"/>
     </row>
     <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
@@ -4381,7 +4309,7 @@
       <c r="F6" s="13">
         <v>401088.37725999998</v>
       </c>
-      <c r="G6" s="47"/>
+      <c r="G6" s="53"/>
     </row>
     <row r="7" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
@@ -4413,7 +4341,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4465,7 +4393,7 @@
       <c r="F2" s="13">
         <v>2</v>
       </c>
-      <c r="G2" s="54" t="s">
+      <c r="G2" s="60" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4488,7 +4416,7 @@
       <c r="F3" s="13">
         <v>299</v>
       </c>
-      <c r="G3" s="54"/>
+      <c r="G3" s="60"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="23" t="s">
@@ -4509,7 +4437,7 @@
       <c r="F4" s="13">
         <v>99</v>
       </c>
-      <c r="G4" s="54"/>
+      <c r="G4" s="60"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -4530,7 +4458,7 @@
       <c r="F5" s="13">
         <v>861</v>
       </c>
-      <c r="G5" s="54"/>
+      <c r="G5" s="60"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="23" t="s">
@@ -4551,7 +4479,7 @@
       <c r="F6" s="13">
         <v>496</v>
       </c>
-      <c r="G6" s="54"/>
+      <c r="G6" s="60"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>

</xml_diff>

<commit_message>
changed email to every 30 seconds
</commit_message>
<xml_diff>
--- a/Data Sets (Excels)/Data (1) (3).xlsx
+++ b/Data Sets (Excels)/Data (1) (3).xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="224" documentId="8_{B116884D-3ADB-43C2-93BC-1D797EACA0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{943D6497-6BCF-4B73-B9E2-25E97ADDCFCE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="4" activeTab="10" xr2:uid="{01528FDC-71FA-430E-A617-D3435C6CD15B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="4" activeTab="8" xr2:uid="{01528FDC-71FA-430E-A617-D3435C6CD15B}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="1" r:id="rId1"/>
@@ -1243,6 +1243,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="18" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1273,16 +1283,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="38" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{6E9C2E63-9F6E-43C0-BFCD-2DC1E9F19C6C}"/>
@@ -1303,10 +1303,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1670,7 +1666,7 @@
       <c r="F2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="67" t="s">
         <v>8</v>
       </c>
       <c r="M2" s="8">
@@ -1699,7 +1695,7 @@
       <c r="F3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="58"/>
+      <c r="G3" s="68"/>
       <c r="M3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1726,7 +1722,7 @@
       <c r="F4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="58"/>
+      <c r="G4" s="68"/>
       <c r="M4" s="4">
         <v>28.360250000000001</v>
       </c>
@@ -1753,7 +1749,7 @@
       <c r="F5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="58"/>
+      <c r="G5" s="68"/>
       <c r="M5" s="4">
         <v>1.7284000000000002</v>
       </c>
@@ -1780,7 +1776,7 @@
       <c r="F6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="58"/>
+      <c r="G6" s="68"/>
       <c r="M6" s="4">
         <v>2133.6398300000005</v>
       </c>
@@ -1865,7 +1861,7 @@
       <c r="F9" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="58" t="s">
+      <c r="G9" s="68" t="s">
         <v>20</v>
       </c>
       <c r="M9" s="4">
@@ -1894,7 +1890,7 @@
       <c r="F10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="58"/>
+      <c r="G10" s="68"/>
       <c r="M10" s="4">
         <v>1193.19</v>
       </c>
@@ -1921,7 +1917,7 @@
       <c r="F11" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="58"/>
+      <c r="G11" s="68"/>
       <c r="M11" s="4">
         <v>14.73</v>
       </c>
@@ -1948,7 +1944,7 @@
       <c r="F12" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="58"/>
+      <c r="G12" s="68"/>
       <c r="M12" s="4">
         <v>52</v>
       </c>
@@ -1975,7 +1971,7 @@
       <c r="F13" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="59" t="s">
+      <c r="G13" s="69" t="s">
         <v>25</v>
       </c>
       <c r="M13" s="4">
@@ -2004,7 +2000,7 @@
       <c r="F14" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="59"/>
+      <c r="G14" s="69"/>
       <c r="M14" s="4">
         <v>0</v>
       </c>
@@ -2031,7 +2027,7 @@
       <c r="F15" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="59"/>
+      <c r="G15" s="69"/>
       <c r="M15" s="4">
         <v>38.119999999999997</v>
       </c>
@@ -2058,7 +2054,7 @@
       <c r="F16" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="53" t="s">
+      <c r="G16" s="63" t="s">
         <v>30</v>
       </c>
       <c r="M16" s="4" t="s">
@@ -2087,7 +2083,7 @@
       <c r="F17" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="53"/>
+      <c r="G17" s="63"/>
       <c r="M17" s="4">
         <v>0</v>
       </c>
@@ -2114,7 +2110,7 @@
       <c r="F18" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="53"/>
+      <c r="G18" s="63"/>
       <c r="M18" s="4">
         <v>0</v>
       </c>
@@ -2141,7 +2137,7 @@
       <c r="F19" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="53"/>
+      <c r="G19" s="63"/>
       <c r="M19" s="4">
         <v>0</v>
       </c>
@@ -2168,7 +2164,7 @@
       <c r="F20" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="60" t="s">
+      <c r="G20" s="70" t="s">
         <v>36</v>
       </c>
       <c r="M20" s="4">
@@ -2197,7 +2193,7 @@
       <c r="F21" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="60"/>
+      <c r="G21" s="70"/>
       <c r="M21" s="4">
         <v>0</v>
       </c>
@@ -2224,7 +2220,7 @@
       <c r="F22" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="60"/>
+      <c r="G22" s="70"/>
       <c r="M22" s="4">
         <v>0</v>
       </c>
@@ -2251,7 +2247,7 @@
       <c r="F23" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="60"/>
+      <c r="G23" s="70"/>
       <c r="M23" s="4">
         <v>0</v>
       </c>
@@ -2278,7 +2274,7 @@
       <c r="F24" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="60"/>
+      <c r="G24" s="70"/>
       <c r="M24" s="4">
         <v>0</v>
       </c>
@@ -2305,7 +2301,7 @@
       <c r="F25" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="G25" s="53" t="s">
+      <c r="G25" s="63" t="s">
         <v>42</v>
       </c>
       <c r="M25" s="4">
@@ -2334,7 +2330,7 @@
       <c r="F26" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="53"/>
+      <c r="G26" s="63"/>
       <c r="M26" s="4">
         <v>144.52000000000001</v>
       </c>
@@ -2361,7 +2357,7 @@
       <c r="F27" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G27" s="53"/>
+      <c r="G27" s="63"/>
       <c r="M27" s="4">
         <v>518.64</v>
       </c>
@@ -2388,7 +2384,7 @@
       <c r="F28" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G28" s="53"/>
+      <c r="G28" s="63"/>
       <c r="M28" s="4">
         <v>667.57999999999993</v>
       </c>
@@ -2415,7 +2411,7 @@
       <c r="F29" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G29" s="53"/>
+      <c r="G29" s="63"/>
       <c r="M29" s="4">
         <v>148.94</v>
       </c>
@@ -2572,7 +2568,7 @@
       <c r="F35" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="G35" s="54" t="s">
+      <c r="G35" s="64" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2596,7 +2592,7 @@
       <c r="F36" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G36" s="55"/>
+      <c r="G36" s="65"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="5">
@@ -2618,7 +2614,7 @@
       <c r="F37" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="G37" s="56"/>
+      <c r="G37" s="66"/>
     </row>
     <row r="38" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="H38" s="1"/>
@@ -2840,7 +2836,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G7" s="54" t="s">
+      <c r="G7" s="64" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2864,7 +2860,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G8" s="55"/>
+      <c r="G8" s="65"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="24" t="s">
@@ -2886,7 +2882,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="G9" s="56"/>
+      <c r="G9" s="66"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H10" s="1"/>
@@ -2922,7 +2918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD8AEB7-D2E8-4525-A681-2676EB3834C0}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -2948,7 +2944,7 @@
       <c r="E1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="57" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2956,23 +2952,23 @@
       <c r="A2" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="63">
+      <c r="B2" s="53">
         <f xml:space="preserve"> 20 - SUM('GHG (Uniform Units)'!B2:B10) /'Production and Facility Info'!B6 / 160000</f>
         <v>11.20802781984602</v>
       </c>
-      <c r="C2" s="63">
+      <c r="C2" s="53">
         <f xml:space="preserve"> 20 - SUM('GHG (Uniform Units)'!C2:C10) /'Production and Facility Info'!C6 / 160000</f>
         <v>-0.49515721093749576</v>
       </c>
-      <c r="D2" s="63">
+      <c r="D2" s="53">
         <f xml:space="preserve"> 20 - SUM('GHG (Uniform Units)'!D2:D10) /'Production and Facility Info'!D6 / 160000</f>
         <v>15.543873163707492</v>
       </c>
-      <c r="E2" s="63">
+      <c r="E2" s="53">
         <f xml:space="preserve"> 20 - SUM('GHG (Uniform Units)'!E2:E10) /'Production and Facility Info'!E6 / 160000</f>
         <v>15.014786223591548</v>
       </c>
-      <c r="F2" s="69">
+      <c r="F2" s="59">
         <f>AVERAGE(B2:E2)</f>
         <v>10.31788249905189</v>
       </c>
@@ -2981,23 +2977,23 @@
       <c r="A3" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="64">
+      <c r="B3" s="54">
         <f>20 -  Energy!B4 /'Production and Facility Info'!B6 / 1</f>
         <v>12.815443517829927</v>
       </c>
-      <c r="C3" s="64">
-        <v>0</v>
-      </c>
-      <c r="D3" s="64">
+      <c r="C3" s="54">
+        <v>0</v>
+      </c>
+      <c r="D3" s="54">
         <f>20 -  Energy!D4 /'Production and Facility Info'!D6 / 1</f>
         <v>14.731884324999999</v>
       </c>
-      <c r="E3" s="64">
+      <c r="E3" s="54">
         <f>20 -  Energy!E4 /'Production and Facility Info'!E6 / 1</f>
         <v>14.044366197183098</v>
       </c>
-      <c r="F3" s="70">
-        <f t="shared" ref="F3:F7" si="0">AVERAGE(B3:E3)</f>
+      <c r="F3" s="60">
+        <f t="shared" ref="F3:F6" si="0">AVERAGE(B3:E3)</f>
         <v>10.397923510003256</v>
       </c>
     </row>
@@ -3005,22 +3001,22 @@
       <c r="A4" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="64">
+      <c r="B4" s="54">
         <f xml:space="preserve"> 20 - (SUM('Water (Uniform Units)'!B2:B3) + 1000000 * 'Water (Uniform Units)'!B5) / 'Production and Facility Info'!B6 / 200000</f>
         <v>6.7499008264462841</v>
       </c>
-      <c r="C4" s="64">
+      <c r="C4" s="54">
         <f xml:space="preserve"> 20 - (SUM('Water (Uniform Units)'!C2:C3) + 1000000 * 'Water (Uniform Units)'!C5) / 'Production and Facility Info'!C6 / 200000</f>
         <v>14.969972727272728</v>
       </c>
-      <c r="D4" s="64">
-        <v>0</v>
-      </c>
-      <c r="E4" s="64">
+      <c r="D4" s="54">
+        <v>0</v>
+      </c>
+      <c r="E4" s="54">
         <f xml:space="preserve"> 20 - (SUM('Water (Uniform Units)'!E2:E3) + 1000000 * 'Water (Uniform Units)'!E5) / 'Production and Facility Info'!E6 / 200000</f>
         <v>19.858380281690142</v>
       </c>
-      <c r="F4" s="70">
+      <c r="F4" s="60">
         <f t="shared" si="0"/>
         <v>10.394563458852289</v>
       </c>
@@ -3029,22 +3025,22 @@
       <c r="A5" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="64">
-        <v>0</v>
-      </c>
-      <c r="C5" s="64">
+      <c r="B5" s="54">
+        <v>0</v>
+      </c>
+      <c r="C5" s="54">
         <f>20 - (Waste!C5-Waste!C6)/'Production and Facility Info'!C6 / 250</f>
         <v>10.343636363636364</v>
       </c>
-      <c r="D5" s="64">
+      <c r="D5" s="54">
         <f>20 - (Waste!D5-Waste!D6)/'Production and Facility Info'!D6 / 250</f>
         <v>11.038861312500002</v>
       </c>
-      <c r="E5" s="64">
+      <c r="E5" s="54">
         <f>20 - (Waste!E5-Waste!E6)/'Production and Facility Info'!E6 / 250</f>
         <v>19.693256338028171</v>
       </c>
-      <c r="F5" s="70">
+      <c r="F5" s="60">
         <f t="shared" si="0"/>
         <v>10.268938503541134</v>
       </c>
@@ -3053,23 +3049,23 @@
       <c r="A6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="65">
+      <c r="B6" s="55">
         <f>20 - (Spills!B3+Spills!B5-Spills!B6)/'Production and Facility Info'!B6 / 2.5</f>
         <v>1.6859504132231429</v>
       </c>
-      <c r="C6" s="65">
+      <c r="C6" s="55">
         <f>20 - (Spills!C3+Spills!C5-Spills!C6)/'Production and Facility Info'!C6 / 2.5</f>
         <v>0</v>
       </c>
-      <c r="D6" s="65">
+      <c r="D6" s="55">
         <f>20 - (Spills!D3+Spills!D5-Spills!D6)/'Production and Facility Info'!D6 / 2.5</f>
         <v>20</v>
       </c>
-      <c r="E6" s="65">
+      <c r="E6" s="55">
         <f>20 - (Spills!E3+Spills!E5-Spills!E6)/'Production and Facility Info'!E6 / 2.5</f>
         <v>20</v>
       </c>
-      <c r="F6" s="71">
+      <c r="F6" s="61">
         <f t="shared" si="0"/>
         <v>10.421487603305785</v>
       </c>
@@ -3078,23 +3074,23 @@
       <c r="A7" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="66">
+      <c r="B7" s="56">
         <f>SUM(B2:B6)</f>
         <v>32.459322577345375</v>
       </c>
-      <c r="C7" s="66">
+      <c r="C7" s="56">
         <f t="shared" ref="C7:E7" si="1">SUM(C2:C6)</f>
         <v>24.818451879971597</v>
       </c>
-      <c r="D7" s="66">
+      <c r="D7" s="56">
         <f t="shared" si="1"/>
         <v>61.314618801207494</v>
       </c>
-      <c r="E7" s="68">
+      <c r="E7" s="58">
         <f t="shared" si="1"/>
         <v>88.610789040492961</v>
       </c>
-      <c r="F7" s="72">
+      <c r="F7" s="62">
         <f>AVERAGE(B7:E7)</f>
         <v>51.80079557475436</v>
       </c>
@@ -3211,7 +3207,7 @@
       <c r="F2" s="12">
         <v>13228.247138200219</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="67" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3234,7 +3230,7 @@
       <c r="F3" s="13">
         <v>1059.88886</v>
       </c>
-      <c r="G3" s="58"/>
+      <c r="G3" s="68"/>
     </row>
     <row r="4" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
@@ -3255,7 +3251,7 @@
       <c r="F4" s="13">
         <v>1704.4953379226879</v>
       </c>
-      <c r="G4" s="58"/>
+      <c r="G4" s="68"/>
     </row>
     <row r="5" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
@@ -3276,7 +3272,7 @@
       <c r="F5" s="13">
         <v>21.443267097804</v>
       </c>
-      <c r="G5" s="58"/>
+      <c r="G5" s="68"/>
     </row>
     <row r="6" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
@@ -3297,7 +3293,7 @@
       <c r="F6" s="13">
         <v>16014.07460322071</v>
       </c>
-      <c r="G6" s="58"/>
+      <c r="G6" s="68"/>
     </row>
     <row r="7" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
@@ -3364,7 +3360,7 @@
       <c r="F9" s="13">
         <v>98507.619583200998</v>
       </c>
-      <c r="G9" s="58" t="s">
+      <c r="G9" s="68" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3387,7 +3383,7 @@
       <c r="F10" s="13">
         <v>48527.770748369003</v>
       </c>
-      <c r="G10" s="58"/>
+      <c r="G10" s="68"/>
     </row>
     <row r="11" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
@@ -3408,7 +3404,7 @@
       <c r="F11" s="13">
         <v>2700.809945126</v>
       </c>
-      <c r="G11" s="58"/>
+      <c r="G11" s="68"/>
     </row>
     <row r="12" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
@@ -3429,7 +3425,7 @@
       <c r="F12" s="13">
         <v>1507.8624917509999</v>
       </c>
-      <c r="G12" s="58"/>
+      <c r="G12" s="68"/>
     </row>
     <row r="13" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
@@ -3518,7 +3514,7 @@
         <f>GHG!F2 * 1000</f>
         <v>13228247.138200218</v>
       </c>
-      <c r="G2" s="61" t="s">
+      <c r="G2" s="71" t="s">
         <v>68</v>
       </c>
     </row>
@@ -3546,7 +3542,7 @@
         <f>GHG!F3 * 1000</f>
         <v>1059888.8600000001</v>
       </c>
-      <c r="G3" s="62"/>
+      <c r="G3" s="72"/>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="19" t="s">
@@ -3572,7 +3568,7 @@
         <f>GHG!F4 * 1000</f>
         <v>1704495.3379226879</v>
       </c>
-      <c r="G4" s="62"/>
+      <c r="G4" s="72"/>
     </row>
     <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="19" t="s">
@@ -3598,7 +3594,7 @@
         <f>GHG!F5 * 1000</f>
         <v>21443.267097804001</v>
       </c>
-      <c r="G5" s="62"/>
+      <c r="G5" s="72"/>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="19" t="s">
@@ -3624,7 +3620,7 @@
         <f>GHG!F6 * 1000</f>
         <v>16014074.603220711</v>
       </c>
-      <c r="G6" s="62"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="21" t="s">
@@ -3645,7 +3641,7 @@
       <c r="F7" s="49">
         <v>98507.619583200998</v>
       </c>
-      <c r="G7" s="62" t="s">
+      <c r="G7" s="72" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3668,7 +3664,7 @@
       <c r="F8" s="49">
         <v>48527.770748369003</v>
       </c>
-      <c r="G8" s="62"/>
+      <c r="G8" s="72"/>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="19" t="s">
@@ -3689,7 +3685,7 @@
       <c r="F9" s="49">
         <v>2700.809945126</v>
       </c>
-      <c r="G9" s="62"/>
+      <c r="G9" s="72"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="19" t="s">
@@ -3710,7 +3706,7 @@
       <c r="F10" s="52">
         <v>1507.8624917509999</v>
       </c>
-      <c r="G10" s="62"/>
+      <c r="G10" s="72"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
@@ -3796,7 +3792,7 @@
       <c r="F2" s="13">
         <v>198.74997016</v>
       </c>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="69" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3819,7 +3815,7 @@
       <c r="F3" s="13">
         <v>7.3924214342898988</v>
       </c>
-      <c r="G3" s="59"/>
+      <c r="G3" s="69"/>
     </row>
     <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
@@ -3840,7 +3836,7 @@
       <c r="F4" s="13">
         <v>206.1423915942899</v>
       </c>
-      <c r="G4" s="59"/>
+      <c r="G4" s="69"/>
     </row>
     <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
@@ -3925,7 +3921,7 @@
       <c r="F2" s="13">
         <v>9.2238950000000006</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="63" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3948,7 +3944,7 @@
       <c r="F3" s="13">
         <v>52.633552000000002</v>
       </c>
-      <c r="G3" s="53"/>
+      <c r="G3" s="63"/>
     </row>
     <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="23" t="s">
@@ -3969,7 +3965,7 @@
       <c r="F4" s="13">
         <v>74.024124999999998</v>
       </c>
-      <c r="G4" s="53"/>
+      <c r="G4" s="63"/>
     </row>
     <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -3990,7 +3986,7 @@
       <c r="F5" s="13">
         <v>129.48417890000002</v>
       </c>
-      <c r="G5" s="53"/>
+      <c r="G5" s="63"/>
     </row>
     <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
@@ -4071,7 +4067,7 @@
         <f>Water!F2 * 1000000</f>
         <v>9223895</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="63" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4099,7 +4095,7 @@
         <f>Water!F3 * 1000000</f>
         <v>52633552</v>
       </c>
-      <c r="G3" s="53"/>
+      <c r="G3" s="63"/>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="23" t="s">
@@ -4125,7 +4121,7 @@
         <f>Water!F4 * 1000000</f>
         <v>74024125</v>
       </c>
-      <c r="G4" s="53"/>
+      <c r="G4" s="63"/>
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="23" t="s">
@@ -4146,7 +4142,7 @@
       <c r="F5" s="13">
         <v>129.48417890000002</v>
       </c>
-      <c r="G5" s="53"/>
+      <c r="G5" s="63"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
@@ -4223,7 +4219,7 @@
       <c r="F2" s="13">
         <v>78599.760600000009</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="63" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4246,7 +4242,7 @@
       <c r="F3" s="13">
         <v>322488.61666</v>
       </c>
-      <c r="G3" s="53"/>
+      <c r="G3" s="63"/>
     </row>
     <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
@@ -4267,7 +4263,7 @@
       <c r="F4" s="13">
         <v>265507.54095000005</v>
       </c>
-      <c r="G4" s="53"/>
+      <c r="G4" s="63"/>
     </row>
     <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
@@ -4288,7 +4284,7 @@
       <c r="F5" s="13">
         <v>666595.91821000003</v>
       </c>
-      <c r="G5" s="53"/>
+      <c r="G5" s="63"/>
     </row>
     <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
@@ -4309,7 +4305,7 @@
       <c r="F6" s="13">
         <v>401088.37725999998</v>
       </c>
-      <c r="G6" s="53"/>
+      <c r="G6" s="63"/>
     </row>
     <row r="7" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
@@ -4340,8 +4336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B326DB89-EB0C-40D8-9CBF-5F3D7B0A1993}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4393,7 +4389,7 @@
       <c r="F2" s="13">
         <v>2</v>
       </c>
-      <c r="G2" s="60" t="s">
+      <c r="G2" s="70" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4416,7 +4412,7 @@
       <c r="F3" s="13">
         <v>299</v>
       </c>
-      <c r="G3" s="60"/>
+      <c r="G3" s="70"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="23" t="s">
@@ -4437,7 +4433,7 @@
       <c r="F4" s="13">
         <v>99</v>
       </c>
-      <c r="G4" s="60"/>
+      <c r="G4" s="70"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -4458,7 +4454,7 @@
       <c r="F5" s="13">
         <v>861</v>
       </c>
-      <c r="G5" s="60"/>
+      <c r="G5" s="70"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="23" t="s">
@@ -4479,7 +4475,7 @@
       <c r="F6" s="13">
         <v>496</v>
       </c>
-      <c r="G6" s="60"/>
+      <c r="G6" s="70"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>

</xml_diff>